<commit_message>
Q2 excel file changed v1 of Q2 removed
</commit_message>
<xml_diff>
--- a/IE407-Q2-v2.xlsx
+++ b/IE407-Q2-v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1028f8d26f624cd18d39-my.sharepoint.com/personal/e246801_metu_edu_tr/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{43E6439F-3F46-4443-93EE-E9BB05D44667}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B59F4456-D29F-458E-B915-92BC2D626BA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{29C75357-6D86-4F34-87D3-5ABA805A4EC9}"/>
   </bookViews>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1862" uniqueCount="1166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1867" uniqueCount="1170">
   <si>
     <t>INDICES</t>
   </si>
@@ -3607,6 +3607,18 @@
   </si>
   <si>
     <t>used for objective function</t>
+  </si>
+  <si>
+    <t>Money Gained</t>
+  </si>
+  <si>
+    <t>Money Gained Per product</t>
+  </si>
+  <si>
+    <t>Total Gain</t>
+  </si>
+  <si>
+    <t>Money Gained per shelf</t>
   </si>
 </sst>
 </file>
@@ -3678,7 +3690,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="23">
+  <borders count="27">
     <border>
       <left/>
       <right/>
@@ -3946,12 +3958,60 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="59">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
@@ -4069,6 +4129,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4104,10 +4168,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="OpenSolver1">
+        <xdr:cNvPr id="40" name="OpenSolver1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BECCAB99-9C4D-424C-9948-849D3B918458}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F71AF40D-C38D-4E1B-BC05-5FB74E9AC844}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4192,10 +4256,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="OpenSolver2">
+        <xdr:cNvPr id="41" name="OpenSolver2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{960B0994-F036-4707-8AFF-499FBFC05B33}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{667D5C69-43F7-47CE-854F-45FCEB357439}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4280,10 +4344,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="4" name="OpenSolver3">
+        <xdr:cNvPr id="42" name="OpenSolver3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F396E916-0186-44C3-88AF-33B27241D5B5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2968F20C-E26D-43A1-A8D7-D657276497EA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4368,10 +4432,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="OpenSolver4">
+        <xdr:cNvPr id="43" name="OpenSolver4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26048256-20E1-4C59-8760-BEC3883CF779}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66651AEE-1500-4269-AF8A-1753BF902079}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4456,10 +4520,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="OpenSolver5">
+        <xdr:cNvPr id="44" name="OpenSolver5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F04332CE-B091-4038-80A5-73AC1876CA5E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A36E8F17-8786-401A-A6FA-C6BA91CE9267}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4538,10 +4602,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="7" name="OpenSolver6">
+        <xdr:cNvPr id="45" name="OpenSolver6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{68D2BAD5-632A-4BDE-8D37-01703A26518A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB6317E0-F7A5-46C9-A5C5-08A2541A1BCC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4631,10 +4695,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="8" name="OpenSolver7">
+        <xdr:cNvPr id="46" name="OpenSolver7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A20E9D7B-8D59-448C-AED6-241E07420EDF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6986BD4F-25E9-484D-ABBF-EFBAA1B5C31E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4713,10 +4777,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="9" name="OpenSolver8">
+        <xdr:cNvPr id="47" name="OpenSolver8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A2326FCA-2571-4C00-8935-EAF1BAF5EC09}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FDA1227-529A-4CFC-985B-24FBD3BA5932}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4798,16 +4862,16 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="10" name="OpenSolver9">
+        <xdr:cNvPr id="48" name="OpenSolver9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EE3CB8E7-5CD6-4ADC-B56F-7C08FF9D318E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B55DE01-2D26-42F9-9B4B-7F9571F321A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="8" idx="3"/>
-          <a:endCxn id="9" idx="1"/>
+          <a:stCxn id="46" idx="3"/>
+          <a:endCxn id="47" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -4859,10 +4923,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="11" name="OpenSolver10">
+        <xdr:cNvPr id="49" name="OpenSolver10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAFAF528-D3EA-4583-BE24-44E0B28C2A82}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32A459F0-EB74-4F3C-85E9-774041A8838C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4946,10 +5010,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="12" name="OpenSolver11">
+        <xdr:cNvPr id="50" name="OpenSolver11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EC61168E-A26F-4571-8355-7EC8AF4EA530}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6383258A-88E2-458D-9C08-CF604E47E79E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5028,10 +5092,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="13" name="OpenSolver12">
+        <xdr:cNvPr id="51" name="OpenSolver12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7AC7CE0E-792E-4D11-BD88-34EF910388AF}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE6DFFDF-4DCD-4102-8934-154DE933088B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5113,16 +5177,16 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="14" name="OpenSolver13">
+        <xdr:cNvPr id="52" name="OpenSolver13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FD4A989D-03B0-40E1-9E26-3D9DC85152CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA74D4C7-9381-47D6-A532-17D9315753E6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="12" idx="3"/>
-          <a:endCxn id="13" idx="1"/>
+          <a:stCxn id="50" idx="3"/>
+          <a:endCxn id="51" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5174,10 +5238,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="15" name="OpenSolver14">
+        <xdr:cNvPr id="53" name="OpenSolver14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{116EA6F6-067E-45B5-BC9D-B650EF601F0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1BF2760-7A9F-46B5-8203-C7AD0CB3692A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5261,10 +5325,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="16" name="OpenSolver15">
+        <xdr:cNvPr id="54" name="OpenSolver15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{215AAE4F-27A4-440A-8985-45DA37E4AA16}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A992895-244B-4807-8252-01C2A8886D85}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5343,10 +5407,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="17" name="OpenSolver16">
+        <xdr:cNvPr id="55" name="OpenSolver16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A449F3B6-DC8A-4DD8-A641-E8907449AC5C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF8A67CD-E442-461B-9759-C2A88853F295}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5428,16 +5492,16 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="18" name="OpenSolver17">
+        <xdr:cNvPr id="56" name="OpenSolver17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDE5B852-01D7-4D40-A9C0-60734C7A01C7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CC932A7-1F42-44B2-8772-3A7D714DFF56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="16" idx="3"/>
-          <a:endCxn id="17" idx="1"/>
+          <a:stCxn id="54" idx="3"/>
+          <a:endCxn id="55" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5489,10 +5553,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="19" name="OpenSolver18">
+        <xdr:cNvPr id="57" name="OpenSolver18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2F7A74BB-3ED5-47DB-805A-C517A1FAEEC1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21878EA8-4CDC-4DC7-B862-12C9BA0BD059}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5576,10 +5640,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="20" name="OpenSolver19">
+        <xdr:cNvPr id="58" name="OpenSolver19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{41F50D52-044B-425E-A106-686EE3A022B9}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA887D8F-62D9-4AE9-BE79-C3467B26CD65}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5658,10 +5722,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="21" name="OpenSolver20">
+        <xdr:cNvPr id="59" name="OpenSolver20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9BBB9194-7FB2-40D7-8485-D34B2AC3418A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE082AA7-8D5C-45F9-853C-8196DF2DCC51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5743,16 +5807,16 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="22" name="OpenSolver21">
+        <xdr:cNvPr id="60" name="OpenSolver21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B38BBF25-E786-49C9-B5CD-DA7B88D51C9F}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAA25DA6-32D5-48F8-A068-AAF0522D71F8}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="20" idx="3"/>
-          <a:endCxn id="21" idx="1"/>
+          <a:stCxn id="58" idx="3"/>
+          <a:endCxn id="59" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -5804,10 +5868,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="23" name="OpenSolver22">
+        <xdr:cNvPr id="61" name="OpenSolver22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{36A90B40-9C85-4A28-9860-75128B4E2C62}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC6EF0B8-A0F4-415F-BAE1-6CC58E8C9F91}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5891,10 +5955,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="24" name="OpenSolver23">
+        <xdr:cNvPr id="62" name="OpenSolver23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{91CBF10F-09FC-4CB4-80A7-12316C64D980}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C369C158-BA79-437F-B0D5-7746A568A04B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5973,10 +6037,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="25" name="OpenSolver24">
+        <xdr:cNvPr id="63" name="OpenSolver24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BC2D3FED-376E-40BA-9AFE-B7C95122E34D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B106CC3-CE5A-4713-8647-476AD757273E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6058,16 +6122,16 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="26" name="OpenSolver25">
+        <xdr:cNvPr id="64" name="OpenSolver25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{7FE66ABD-1C29-4F68-9414-D260530EFFAC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95681D30-6657-4FB2-AEBF-BDFC09770C85}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="24" idx="3"/>
-          <a:endCxn id="25" idx="1"/>
+          <a:stCxn id="62" idx="3"/>
+          <a:endCxn id="63" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -6119,10 +6183,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="27" name="OpenSolver26">
+        <xdr:cNvPr id="65" name="OpenSolver26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3A6116E2-110A-4285-8ABC-7DF45AF87EC5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99ED5F60-C731-4BC3-B279-DF4F089511DD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6206,10 +6270,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="28" name="OpenSolver27">
+        <xdr:cNvPr id="66" name="OpenSolver27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{11C30E3F-0598-4FCC-BAFC-0BF06945FAA6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42045BA8-DB7B-48A1-AA6D-A09E8C17FC51}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6288,10 +6352,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="29" name="OpenSolver28">
+        <xdr:cNvPr id="67" name="OpenSolver28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E1E25E00-BE42-4D74-B518-94596EFA4AD0}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1B1CD39-6E2E-4A53-8EC3-1D58940646A7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6373,16 +6437,16 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="30" name="OpenSolver29">
+        <xdr:cNvPr id="68" name="OpenSolver29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0D209F7A-F1FE-40FA-81A6-9D0BAF32CDB7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E44D99-74F7-4063-A565-3A480442C770}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="28" idx="3"/>
-          <a:endCxn id="29" idx="1"/>
+          <a:stCxn id="66" idx="3"/>
+          <a:endCxn id="67" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
@@ -6434,10 +6498,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="31" name="OpenSolver30">
+        <xdr:cNvPr id="69" name="OpenSolver30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{25E03FF5-E0D3-4153-AF9F-0401F6165760}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{645165AD-02BF-4CFB-BC02-4DD68CBF793B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6521,10 +6585,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="32" name="OpenSolver31">
+        <xdr:cNvPr id="70" name="OpenSolver31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5AEE190A-8529-4EFF-A854-23BD6DFDEE08}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53E937B6-B3EE-4857-ABAE-E4B28536479B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6603,10 +6667,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="33" name="OpenSolver32">
+        <xdr:cNvPr id="71" name="OpenSolver32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{26C12812-B8F8-4348-946B-41330610C09C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4672B8E0-170D-4F61-929A-02874B1B0B64}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6696,10 +6760,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="34" name="OpenSolver33">
+        <xdr:cNvPr id="72" name="OpenSolver33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB455ADE-D2E8-4881-A009-D2C20004E899}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48E9FAB7-5B97-484C-B30F-67834FBC8B4E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6778,10 +6842,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="35" name="OpenSolver34">
+        <xdr:cNvPr id="73" name="OpenSolver34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{62ED9C17-7F4A-4111-BD59-AD7B2890FCF5}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D4FA2AA-BA98-4368-BF34-F96088B014C1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6871,10 +6935,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="36" name="OpenSolver35">
+        <xdr:cNvPr id="74" name="OpenSolver35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99B86859-543E-4C57-A65D-7B2AD3D057F7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDCEC243-56E8-4221-A7CF-A1463C65E07B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6953,10 +7017,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="37" name="OpenSolver36">
+        <xdr:cNvPr id="75" name="OpenSolver36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED81621D-C155-40D3-9DEF-826284C42951}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F080CB5-4934-4356-9BA9-CAC593587009}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7046,10 +7110,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="38" name="OpenSolver37">
+        <xdr:cNvPr id="76" name="OpenSolver37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{939DA02F-DE2C-4A96-8A15-3B45BA732D1D}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{382F5A23-0D2D-4047-91B5-A4D998750FBD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7128,10 +7192,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="39" name="OpenSolver38">
+        <xdr:cNvPr id="77" name="OpenSolver38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9B7FCE64-791C-4F55-8AC7-022D38C13F78}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B79BA49-10D5-4550-B434-C930C7417FB3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -31937,8 +32001,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7930316F-CD20-49E5-A6A0-4C42FB60CBBA}">
   <dimension ref="A1:CM132"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="BU20" sqref="BU20"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="BQ57" sqref="BQ57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -31977,8 +32041,9 @@
     <col min="49" max="54" width="8.88671875" style="1"/>
     <col min="55" max="55" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="56" max="61" width="8.88671875" style="1"/>
-    <col min="62" max="62" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="63" max="68" width="8.88671875" style="1"/>
+    <col min="62" max="62" width="31.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="63" max="67" width="8.88671875" style="1"/>
+    <col min="68" max="68" width="26.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="69" max="69" width="9.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="70" max="16384" width="8.88671875" style="1"/>
   </cols>
@@ -38562,6 +38627,9 @@
       <c r="AD37" s="8"/>
       <c r="AE37" s="8"/>
       <c r="AF37" s="9"/>
+      <c r="BJ37" s="62" t="s">
+        <v>1166</v>
+      </c>
     </row>
     <row r="38" spans="2:81" x14ac:dyDescent="0.3">
       <c r="B38" s="32"/>
@@ -38595,6 +38663,27 @@
       <c r="AD38" s="8"/>
       <c r="AE38" s="8"/>
       <c r="AF38" s="9"/>
+      <c r="BJ38" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="BK38" s="61">
+        <v>1</v>
+      </c>
+      <c r="BL38" s="16">
+        <v>2</v>
+      </c>
+      <c r="BM38" s="16">
+        <v>3</v>
+      </c>
+      <c r="BN38" s="16">
+        <v>4</v>
+      </c>
+      <c r="BO38" s="16">
+        <v>5</v>
+      </c>
+      <c r="BP38" s="60" t="s">
+        <v>1167</v>
+      </c>
     </row>
     <row r="39" spans="2:81" x14ac:dyDescent="0.3">
       <c r="B39" s="7"/>
@@ -38628,6 +38717,33 @@
       <c r="AD39" s="8"/>
       <c r="AE39" s="8"/>
       <c r="AF39" s="9"/>
+      <c r="BJ39" s="16">
+        <v>1</v>
+      </c>
+      <c r="BK39" s="61" cm="1">
+        <f t="array" aca="1" ref="BK39" ca="1">BY6*$C6*$L6*POWER($F6,$O6)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A1),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL39" s="16" cm="1">
+        <f t="array" aca="1" ref="BL39" ca="1">BZ6*$C6*$L6*POWER($F6,$O6)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B1),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM39" s="16" cm="1">
+        <f t="array" aca="1" ref="BM39" ca="1">CA6*$C6*$L6*POWER($F6,$O6)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C1),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN39" s="16" cm="1">
+        <f t="array" aca="1" ref="BN39" ca="1">CB6*$C6*$L6*POWER($F6,$O6)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D1),9))</f>
+        <v>113.84199576606166</v>
+      </c>
+      <c r="BO39" s="16" cm="1">
+        <f t="array" aca="1" ref="BO39" ca="1">CC6*$C6*$L6*POWER($F6,$O6)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E1),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP39" s="1">
+        <f ca="1">SUM(BK39:BO39)</f>
+        <v>113.84199576606166</v>
+      </c>
     </row>
     <row r="40" spans="2:81" x14ac:dyDescent="0.3">
       <c r="B40" s="7"/>
@@ -38661,6 +38777,33 @@
       <c r="AD40" s="8"/>
       <c r="AE40" s="8"/>
       <c r="AF40" s="9"/>
+      <c r="BJ40" s="16">
+        <v>2</v>
+      </c>
+      <c r="BK40" s="61" cm="1">
+        <f t="array" aca="1" ref="BK40" ca="1">BY7*$C7*$L7*POWER($F7,$O7)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A2),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL40" s="16" cm="1">
+        <f t="array" aca="1" ref="BL40" ca="1">BZ7*$C7*$L7*POWER($F7,$O7)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B2),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM40" s="16" cm="1">
+        <f t="array" aca="1" ref="BM40" ca="1">CA7*$C7*$L7*POWER($F7,$O7)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C2),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN40" s="16" cm="1">
+        <f t="array" aca="1" ref="BN40" ca="1">CB7*$C7*$L7*POWER($F7,$O7)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D2),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO40" s="16" cm="1">
+        <f t="array" aca="1" ref="BO40" ca="1">CC7*$C7*$L7*POWER($F7,$O7)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E2),9))</f>
+        <v>31.036911478307196</v>
+      </c>
+      <c r="BP40" s="1">
+        <f t="shared" ref="BP40:BP64" ca="1" si="23">SUM(BK40:BO40)</f>
+        <v>31.036911478307196</v>
+      </c>
     </row>
     <row r="41" spans="2:81" x14ac:dyDescent="0.3">
       <c r="B41" s="10" t="s">
@@ -38696,6 +38839,33 @@
       <c r="AD41" s="8"/>
       <c r="AE41" s="8"/>
       <c r="AF41" s="9"/>
+      <c r="BJ41" s="16">
+        <v>3</v>
+      </c>
+      <c r="BK41" s="61" cm="1">
+        <f t="array" aca="1" ref="BK41" ca="1">BY8*$C8*$L8*POWER($F8,$O8)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A3),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL41" s="16" cm="1">
+        <f t="array" aca="1" ref="BL41" ca="1">BZ8*$C8*$L8*POWER($F8,$O8)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B3),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM41" s="16" cm="1">
+        <f t="array" aca="1" ref="BM41" ca="1">CA8*$C8*$L8*POWER($F8,$O8)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C3),9))</f>
+        <v>194.4787916031315</v>
+      </c>
+      <c r="BN41" s="16" cm="1">
+        <f t="array" aca="1" ref="BN41" ca="1">CB8*$C8*$L8*POWER($F8,$O8)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D3),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO41" s="16" cm="1">
+        <f t="array" aca="1" ref="BO41" ca="1">CC8*$C8*$L8*POWER($F8,$O8)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E3),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP41" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>194.4787916031315</v>
+      </c>
     </row>
     <row r="42" spans="2:81" x14ac:dyDescent="0.3">
       <c r="B42" s="7">
@@ -38733,6 +38903,33 @@
       <c r="AD42" s="8"/>
       <c r="AE42" s="8"/>
       <c r="AF42" s="9"/>
+      <c r="BJ42" s="16">
+        <v>4</v>
+      </c>
+      <c r="BK42" s="61" cm="1">
+        <f t="array" aca="1" ref="BK42" ca="1">BY9*$C9*$L9*POWER($F9,$O9)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A4),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL42" s="16" cm="1">
+        <f t="array" aca="1" ref="BL42" ca="1">BZ9*$C9*$L9*POWER($F9,$O9)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B4),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM42" s="16" cm="1">
+        <f t="array" aca="1" ref="BM42" ca="1">CA9*$C9*$L9*POWER($F9,$O9)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C4),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN42" s="16" cm="1">
+        <f t="array" aca="1" ref="BN42" ca="1">CB9*$C9*$L9*POWER($F9,$O9)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D4),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO42" s="16" cm="1">
+        <f t="array" aca="1" ref="BO42" ca="1">CC9*$C9*$L9*POWER($F9,$O9)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E4),9))</f>
+        <v>15.495618196742795</v>
+      </c>
+      <c r="BP42" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>15.495618196742795</v>
+      </c>
     </row>
     <row r="43" spans="2:81" x14ac:dyDescent="0.3">
       <c r="B43" s="7">
@@ -38770,6 +38967,33 @@
       <c r="AD43" s="8"/>
       <c r="AE43" s="8"/>
       <c r="AF43" s="9"/>
+      <c r="BJ43" s="16">
+        <v>5</v>
+      </c>
+      <c r="BK43" s="61" cm="1">
+        <f t="array" aca="1" ref="BK43" ca="1">BY10*$C10*$L10*POWER($F10,$O10)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A5),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL43" s="16" cm="1">
+        <f t="array" aca="1" ref="BL43" ca="1">BZ10*$C10*$L10*POWER($F10,$O10)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B5),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM43" s="16" cm="1">
+        <f t="array" aca="1" ref="BM43" ca="1">CA10*$C10*$L10*POWER($F10,$O10)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C5),9))</f>
+        <v>1383.6776951677273</v>
+      </c>
+      <c r="BN43" s="16" cm="1">
+        <f t="array" aca="1" ref="BN43" ca="1">CB10*$C10*$L10*POWER($F10,$O10)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D5),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO43" s="16" cm="1">
+        <f t="array" aca="1" ref="BO43" ca="1">CC10*$C10*$L10*POWER($F10,$O10)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E5),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP43" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>1383.6776951677273</v>
+      </c>
     </row>
     <row r="44" spans="2:81" x14ac:dyDescent="0.3">
       <c r="B44" s="7">
@@ -38807,6 +39031,33 @@
       <c r="AD44" s="8"/>
       <c r="AE44" s="8"/>
       <c r="AF44" s="9"/>
+      <c r="BJ44" s="16">
+        <v>6</v>
+      </c>
+      <c r="BK44" s="61" cm="1">
+        <f t="array" aca="1" ref="BK44" ca="1">BY11*$C11*$L11*POWER($F11,$O11)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A6),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL44" s="16" cm="1">
+        <f t="array" aca="1" ref="BL44" ca="1">BZ11*$C11*$L11*POWER($F11,$O11)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B6),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM44" s="16" cm="1">
+        <f t="array" aca="1" ref="BM44" ca="1">CA11*$C11*$L11*POWER($F11,$O11)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C6),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN44" s="16" cm="1">
+        <f t="array" aca="1" ref="BN44" ca="1">CB11*$C11*$L11*POWER($F11,$O11)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D6),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO44" s="16" cm="1">
+        <f t="array" aca="1" ref="BO44" ca="1">CC11*$C11*$L11*POWER($F11,$O11)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E6),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP44" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="2:81" x14ac:dyDescent="0.3">
       <c r="B45" s="7"/>
@@ -38840,6 +39091,33 @@
       <c r="AD45" s="8"/>
       <c r="AE45" s="8"/>
       <c r="AF45" s="9"/>
+      <c r="BJ45" s="16">
+        <v>7</v>
+      </c>
+      <c r="BK45" s="61" cm="1">
+        <f t="array" aca="1" ref="BK45" ca="1">BY12*$C12*$L12*POWER($F12,$O12)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A7),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL45" s="16" cm="1">
+        <f t="array" aca="1" ref="BL45" ca="1">BZ12*$C12*$L12*POWER($F12,$O12)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B7),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM45" s="16" cm="1">
+        <f t="array" aca="1" ref="BM45" ca="1">CA12*$C12*$L12*POWER($F12,$O12)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C7),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN45" s="16" cm="1">
+        <f t="array" aca="1" ref="BN45" ca="1">CB12*$C12*$L12*POWER($F12,$O12)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D7),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO45" s="16" cm="1">
+        <f t="array" aca="1" ref="BO45" ca="1">CC12*$C12*$L12*POWER($F12,$O12)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E7),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP45" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="2:81" x14ac:dyDescent="0.3">
       <c r="B46" s="10" t="s">
@@ -38875,6 +39153,33 @@
       <c r="AD46" s="8"/>
       <c r="AE46" s="8"/>
       <c r="AF46" s="9"/>
+      <c r="BJ46" s="16">
+        <v>8</v>
+      </c>
+      <c r="BK46" s="61" cm="1">
+        <f t="array" aca="1" ref="BK46" ca="1">BY13*$C13*$L13*POWER($F13,$O13)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A8),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL46" s="16" cm="1">
+        <f t="array" aca="1" ref="BL46" ca="1">BZ13*$C13*$L13*POWER($F13,$O13)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B8),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM46" s="16" cm="1">
+        <f t="array" aca="1" ref="BM46" ca="1">CA13*$C13*$L13*POWER($F13,$O13)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C8),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN46" s="16" cm="1">
+        <f t="array" aca="1" ref="BN46" ca="1">CB13*$C13*$L13*POWER($F13,$O13)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D8),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO46" s="16" cm="1">
+        <f t="array" aca="1" ref="BO46" ca="1">CC13*$C13*$L13*POWER($F13,$O13)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E8),9))</f>
+        <v>14.585909370234862</v>
+      </c>
+      <c r="BP46" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>14.585909370234862</v>
+      </c>
     </row>
     <row r="47" spans="2:81" x14ac:dyDescent="0.3">
       <c r="B47" s="7">
@@ -38912,6 +39217,33 @@
       <c r="AD47" s="8"/>
       <c r="AE47" s="8"/>
       <c r="AF47" s="9"/>
+      <c r="BJ47" s="16">
+        <v>9</v>
+      </c>
+      <c r="BK47" s="61" cm="1">
+        <f t="array" aca="1" ref="BK47" ca="1">BY14*$C14*$L14*POWER($F14,$O14)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A9),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL47" s="16" cm="1">
+        <f t="array" aca="1" ref="BL47" ca="1">BZ14*$C14*$L14*POWER($F14,$O14)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B9),9))</f>
+        <v>293.2988134700031</v>
+      </c>
+      <c r="BM47" s="16" cm="1">
+        <f t="array" aca="1" ref="BM47" ca="1">CA14*$C14*$L14*POWER($F14,$O14)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C9),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN47" s="16" cm="1">
+        <f t="array" aca="1" ref="BN47" ca="1">CB14*$C14*$L14*POWER($F14,$O14)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D9),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO47" s="16" cm="1">
+        <f t="array" aca="1" ref="BO47" ca="1">CC14*$C14*$L14*POWER($F14,$O14)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E9),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP47" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>293.2988134700031</v>
+      </c>
     </row>
     <row r="48" spans="2:81" x14ac:dyDescent="0.3">
       <c r="B48" s="7">
@@ -38951,6 +39283,33 @@
       <c r="AF48" s="9"/>
       <c r="AH48" s="8" t="s">
         <v>23</v>
+      </c>
+      <c r="BJ48" s="16">
+        <v>10</v>
+      </c>
+      <c r="BK48" s="61" cm="1">
+        <f t="array" aca="1" ref="BK48" ca="1">BY15*$C15*$L15*POWER($F15,$O15)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A10),9))</f>
+        <v>125.3576818177493</v>
+      </c>
+      <c r="BL48" s="16" cm="1">
+        <f t="array" aca="1" ref="BL48" ca="1">BZ15*$C15*$L15*POWER($F15,$O15)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B10),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM48" s="16" cm="1">
+        <f t="array" aca="1" ref="BM48" ca="1">CA15*$C15*$L15*POWER($F15,$O15)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C10),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN48" s="16" cm="1">
+        <f t="array" aca="1" ref="BN48" ca="1">CB15*$C15*$L15*POWER($F15,$O15)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D10),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO48" s="16" cm="1">
+        <f t="array" aca="1" ref="BO48" ca="1">CC15*$C15*$L15*POWER($F15,$O15)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E10),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP48" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>125.3576818177493</v>
       </c>
     </row>
     <row r="49" spans="1:91" x14ac:dyDescent="0.3">
@@ -38993,6 +39352,33 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6,26+ROWS($A$1:A1))):INDIRECT(ADDRESS(30,26+ROWS($A$1:A1))))</f>
         <v>103</v>
       </c>
+      <c r="BJ49" s="16">
+        <v>11</v>
+      </c>
+      <c r="BK49" s="61" cm="1">
+        <f t="array" aca="1" ref="BK49" ca="1">BY16*$C16*$L16*POWER($F16,$O16)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A11),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL49" s="16" cm="1">
+        <f t="array" aca="1" ref="BL49" ca="1">BZ16*$C16*$L16*POWER($F16,$O16)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B11),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM49" s="16" cm="1">
+        <f t="array" aca="1" ref="BM49" ca="1">CA16*$C16*$L16*POWER($F16,$O16)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C11),9))</f>
+        <v>58.311074113875208</v>
+      </c>
+      <c r="BN49" s="16" cm="1">
+        <f t="array" aca="1" ref="BN49" ca="1">CB16*$C16*$L16*POWER($F16,$O16)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D11),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO49" s="16" cm="1">
+        <f t="array" aca="1" ref="BO49" ca="1">CC16*$C16*$L16*POWER($F16,$O16)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E11),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP49" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>58.311074113875208</v>
+      </c>
     </row>
     <row r="50" spans="1:91" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B50" s="25">
@@ -39034,11 +39420,65 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6,26+ROWS($A$1:A2))):INDIRECT(ADDRESS(30,26+ROWS($A$1:A2))))</f>
         <v>99</v>
       </c>
+      <c r="BJ50" s="16">
+        <v>12</v>
+      </c>
+      <c r="BK50" s="61" cm="1">
+        <f t="array" aca="1" ref="BK50" ca="1">BY17*$C17*$L17*POWER($F17,$O17)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A12),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL50" s="16" cm="1">
+        <f t="array" aca="1" ref="BL50" ca="1">BZ17*$C17*$L17*POWER($F17,$O17)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B12),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM50" s="16" cm="1">
+        <f t="array" aca="1" ref="BM50" ca="1">CA17*$C17*$L17*POWER($F17,$O17)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C12),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN50" s="16" cm="1">
+        <f t="array" aca="1" ref="BN50" ca="1">CB17*$C17*$L17*POWER($F17,$O17)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D12),9))</f>
+        <v>369.11634255085556</v>
+      </c>
+      <c r="BO50" s="16" cm="1">
+        <f t="array" aca="1" ref="BO50" ca="1">CC17*$C17*$L17*POWER($F17,$O17)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E12),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP50" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>369.11634255085556</v>
+      </c>
     </row>
     <row r="51" spans="1:91" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="AH51" s="1">
         <f ca="1">SUM(INDIRECT(ADDRESS(6,26+ROWS($A$1:A3))):INDIRECT(ADDRESS(30,26+ROWS($A$1:A3))))</f>
         <v>78</v>
+      </c>
+      <c r="BJ51" s="16">
+        <v>13</v>
+      </c>
+      <c r="BK51" s="61" cm="1">
+        <f t="array" aca="1" ref="BK51" ca="1">BY18*$C18*$L18*POWER($F18,$O18)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A13),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL51" s="16" cm="1">
+        <f t="array" aca="1" ref="BL51" ca="1">BZ18*$C18*$L18*POWER($F18,$O18)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B13),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM51" s="16" cm="1">
+        <f t="array" aca="1" ref="BM51" ca="1">CA18*$C18*$L18*POWER($F18,$O18)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C13),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN51" s="16" cm="1">
+        <f t="array" aca="1" ref="BN51" ca="1">CB18*$C18*$L18*POWER($F18,$O18)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D13),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO51" s="16" cm="1">
+        <f t="array" aca="1" ref="BO51" ca="1">CC18*$C18*$L18*POWER($F18,$O18)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E13),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP51" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:91" x14ac:dyDescent="0.3">
@@ -39057,6 +39497,33 @@
       <c r="AH52" s="1">
         <f ca="1">SUM(INDIRECT(ADDRESS(6,26+ROWS($A$1:A4))):INDIRECT(ADDRESS(30,26+ROWS($A$1:A4))))</f>
         <v>85</v>
+      </c>
+      <c r="BJ52" s="16">
+        <v>14</v>
+      </c>
+      <c r="BK52" s="61" cm="1">
+        <f t="array" aca="1" ref="BK52" ca="1">BY19*$C19*$L19*POWER($F19,$O19)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A14),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL52" s="16" cm="1">
+        <f t="array" aca="1" ref="BL52" ca="1">BZ19*$C19*$L19*POWER($F19,$O19)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B14),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM52" s="16" cm="1">
+        <f t="array" aca="1" ref="BM52" ca="1">CA19*$C19*$L19*POWER($F19,$O19)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C14),9))</f>
+        <v>1871.9999999999998</v>
+      </c>
+      <c r="BN52" s="16" cm="1">
+        <f t="array" aca="1" ref="BN52" ca="1">CB19*$C19*$L19*POWER($F19,$O19)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D14),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO52" s="16" cm="1">
+        <f t="array" aca="1" ref="BO52" ca="1">CC19*$C19*$L19*POWER($F19,$O19)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E14),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP52" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>1871.9999999999998</v>
       </c>
     </row>
     <row r="53" spans="1:91" x14ac:dyDescent="0.3">
@@ -39074,6 +39541,33 @@
         <f ca="1">SUM(INDIRECT(ADDRESS(6,26+ROWS($A$1:A5))):INDIRECT(ADDRESS(30,26+ROWS($A$1:A5))))</f>
         <v>88</v>
       </c>
+      <c r="BJ53" s="16">
+        <v>15</v>
+      </c>
+      <c r="BK53" s="61" cm="1">
+        <f t="array" aca="1" ref="BK53" ca="1">BY20*$C20*$L20*POWER($F20,$O20)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A15),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL53" s="16" cm="1">
+        <f t="array" aca="1" ref="BL53" ca="1">BZ20*$C20*$L20*POWER($F20,$O20)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B15),9))</f>
+        <v>812.23925749895227</v>
+      </c>
+      <c r="BM53" s="16" cm="1">
+        <f t="array" aca="1" ref="BM53" ca="1">CA20*$C20*$L20*POWER($F20,$O20)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C15),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN53" s="16" cm="1">
+        <f t="array" aca="1" ref="BN53" ca="1">CB20*$C20*$L20*POWER($F20,$O20)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D15),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO53" s="16" cm="1">
+        <f t="array" aca="1" ref="BO53" ca="1">CC20*$C20*$L20*POWER($F20,$O20)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E15),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP53" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>812.23925749895227</v>
+      </c>
     </row>
     <row r="54" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B54" s="7"/>
@@ -39086,6 +39580,33 @@
       </c>
       <c r="I54" s="11"/>
       <c r="J54" s="34"/>
+      <c r="BJ54" s="16">
+        <v>16</v>
+      </c>
+      <c r="BK54" s="61" cm="1">
+        <f t="array" aca="1" ref="BK54" ca="1">BY21*$C21*$L21*POWER($F21,$O21)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A16),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL54" s="16" cm="1">
+        <f t="array" aca="1" ref="BL54" ca="1">BZ21*$C21*$L21*POWER($F21,$O21)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B16),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM54" s="16" cm="1">
+        <f t="array" aca="1" ref="BM54" ca="1">CA21*$C21*$L21*POWER($F21,$O21)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C16),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN54" s="16" cm="1">
+        <f t="array" aca="1" ref="BN54" ca="1">CB21*$C21*$L21*POWER($F21,$O21)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D16),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO54" s="16" cm="1">
+        <f t="array" aca="1" ref="BO54" ca="1">CC21*$C21*$L21*POWER($F21,$O21)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E16),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP54" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:91" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="25" cm="1">
@@ -39101,8 +39622,63 @@
       </c>
       <c r="I55" s="26"/>
       <c r="J55" s="27"/>
-    </row>
-    <row r="56" spans="1:91" ht="16.2" thickBot="1" x14ac:dyDescent="0.35"/>
+      <c r="BJ55" s="16">
+        <v>17</v>
+      </c>
+      <c r="BK55" s="61" cm="1">
+        <f t="array" aca="1" ref="BK55" ca="1">BY22*$C22*$L22*POWER($F22,$O22)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A17),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL55" s="16" cm="1">
+        <f t="array" aca="1" ref="BL55" ca="1">BZ22*$C22*$L22*POWER($F22,$O22)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B17),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM55" s="16" cm="1">
+        <f t="array" aca="1" ref="BM55" ca="1">CA22*$C22*$L22*POWER($F22,$O22)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C17),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN55" s="16" cm="1">
+        <f t="array" aca="1" ref="BN55" ca="1">CB22*$C22*$L22*POWER($F22,$O22)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D17),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO55" s="16" cm="1">
+        <f t="array" aca="1" ref="BO55" ca="1">CC22*$C22*$L22*POWER($F22,$O22)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E17),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP55" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:91" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="BJ56" s="16">
+        <v>18</v>
+      </c>
+      <c r="BK56" s="61" cm="1">
+        <f t="array" aca="1" ref="BK56" ca="1">BY23*$C23*$L23*POWER($F23,$O23)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A18),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL56" s="16" cm="1">
+        <f t="array" aca="1" ref="BL56" ca="1">BZ23*$C23*$L23*POWER($F23,$O23)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B18),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM56" s="16" cm="1">
+        <f t="array" aca="1" ref="BM56" ca="1">CA23*$C23*$L23*POWER($F23,$O23)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C18),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN56" s="16" cm="1">
+        <f t="array" aca="1" ref="BN56" ca="1">CB23*$C23*$L23*POWER($F23,$O23)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D18),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO56" s="16" cm="1">
+        <f t="array" aca="1" ref="BO56" ca="1">CC23*$C23*$L23*POWER($F23,$O23)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E18),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP56" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>0</v>
+      </c>
+    </row>
     <row r="57" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B57" s="2" t="s">
         <v>6</v>
@@ -39166,13 +39742,33 @@
       <c r="BG57" s="8"/>
       <c r="BH57" s="8"/>
       <c r="BI57" s="8"/>
-      <c r="BJ57" s="8"/>
-      <c r="BK57" s="8"/>
-      <c r="BL57" s="8"/>
-      <c r="BM57" s="8"/>
-      <c r="BN57" s="8"/>
-      <c r="BO57" s="8"/>
-      <c r="BP57" s="8"/>
+      <c r="BJ57" s="16">
+        <v>19</v>
+      </c>
+      <c r="BK57" s="61" cm="1">
+        <f t="array" aca="1" ref="BK57" ca="1">BY24*$C24*$L24*POWER($F24,$O24)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A19),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL57" s="16" cm="1">
+        <f t="array" aca="1" ref="BL57" ca="1">BZ24*$C24*$L24*POWER($F24,$O24)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B19),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM57" s="16" cm="1">
+        <f t="array" aca="1" ref="BM57" ca="1">CA24*$C24*$L24*POWER($F24,$O24)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C19),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN57" s="16" cm="1">
+        <f t="array" aca="1" ref="BN57" ca="1">CB24*$C24*$L24*POWER($F24,$O24)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D19),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO57" s="16" cm="1">
+        <f t="array" aca="1" ref="BO57" ca="1">CC24*$C24*$L24*POWER($F24,$O24)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E19),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP57" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>0</v>
+      </c>
       <c r="BQ57" s="8"/>
       <c r="BR57" s="8"/>
       <c r="BS57" s="8"/>
@@ -39258,13 +39854,33 @@
       <c r="BG58" s="8"/>
       <c r="BH58" s="8"/>
       <c r="BI58" s="8"/>
-      <c r="BJ58" s="8"/>
-      <c r="BK58" s="8"/>
-      <c r="BL58" s="8"/>
-      <c r="BM58" s="8"/>
-      <c r="BN58" s="8"/>
-      <c r="BO58" s="8"/>
-      <c r="BP58" s="8"/>
+      <c r="BJ58" s="16">
+        <v>20</v>
+      </c>
+      <c r="BK58" s="61" cm="1">
+        <f t="array" aca="1" ref="BK58" ca="1">BY25*$C25*$L25*POWER($F25,$O25)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A20),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL58" s="16" cm="1">
+        <f t="array" aca="1" ref="BL58" ca="1">BZ25*$C25*$L25*POWER($F25,$O25)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B20),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM58" s="16" cm="1">
+        <f t="array" aca="1" ref="BM58" ca="1">CA25*$C25*$L25*POWER($F25,$O25)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C20),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN58" s="16" cm="1">
+        <f t="array" aca="1" ref="BN58" ca="1">CB25*$C25*$L25*POWER($F25,$O25)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D20),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO58" s="16" cm="1">
+        <f t="array" aca="1" ref="BO58" ca="1">CC25*$C25*$L25*POWER($F25,$O25)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E20),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP58" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>0</v>
+      </c>
       <c r="BQ58" s="8"/>
       <c r="BR58" s="8"/>
       <c r="BS58" s="8"/>
@@ -39350,13 +39966,33 @@
       <c r="BG59" s="8"/>
       <c r="BH59" s="8"/>
       <c r="BI59" s="8"/>
-      <c r="BJ59" s="8"/>
-      <c r="BK59" s="8"/>
-      <c r="BL59" s="8"/>
-      <c r="BM59" s="8"/>
-      <c r="BN59" s="8"/>
-      <c r="BO59" s="8"/>
-      <c r="BP59" s="8"/>
+      <c r="BJ59" s="16">
+        <v>21</v>
+      </c>
+      <c r="BK59" s="61" cm="1">
+        <f t="array" aca="1" ref="BK59" ca="1">BY26*$C26*$L26*POWER($F26,$O26)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A21),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL59" s="16" cm="1">
+        <f t="array" aca="1" ref="BL59" ca="1">BZ26*$C26*$L26*POWER($F26,$O26)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B21),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM59" s="16" cm="1">
+        <f t="array" aca="1" ref="BM59" ca="1">CA26*$C26*$L26*POWER($F26,$O26)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C21),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN59" s="16" cm="1">
+        <f t="array" aca="1" ref="BN59" ca="1">CB26*$C26*$L26*POWER($F26,$O26)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D21),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO59" s="16" cm="1">
+        <f t="array" aca="1" ref="BO59" ca="1">CC26*$C26*$L26*POWER($F26,$O26)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E21),9))</f>
+        <v>186.64177568163981</v>
+      </c>
+      <c r="BP59" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>186.64177568163981</v>
+      </c>
       <c r="BQ59" s="8"/>
       <c r="BR59" s="8"/>
       <c r="BS59" s="8"/>
@@ -39443,13 +40079,33 @@
       <c r="BG60" s="8"/>
       <c r="BH60" s="8"/>
       <c r="BI60" s="8"/>
-      <c r="BJ60" s="8"/>
-      <c r="BK60" s="8"/>
-      <c r="BL60" s="8"/>
-      <c r="BM60" s="8"/>
-      <c r="BN60" s="8"/>
-      <c r="BO60" s="8"/>
-      <c r="BP60" s="8"/>
+      <c r="BJ60" s="16">
+        <v>22</v>
+      </c>
+      <c r="BK60" s="61" cm="1">
+        <f t="array" aca="1" ref="BK60" ca="1">BY27*$C27*$L27*POWER($F27,$O27)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A22),9))</f>
+        <v>53.577862653738528</v>
+      </c>
+      <c r="BL60" s="16" cm="1">
+        <f t="array" aca="1" ref="BL60" ca="1">BZ27*$C27*$L27*POWER($F27,$O27)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B22),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM60" s="16" cm="1">
+        <f t="array" aca="1" ref="BM60" ca="1">CA27*$C27*$L27*POWER($F27,$O27)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C22),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN60" s="16" cm="1">
+        <f t="array" aca="1" ref="BN60" ca="1">CB27*$C27*$L27*POWER($F27,$O27)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D22),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO60" s="16" cm="1">
+        <f t="array" aca="1" ref="BO60" ca="1">CC27*$C27*$L27*POWER($F27,$O27)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E22),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP60" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>53.577862653738528</v>
+      </c>
       <c r="BQ60" s="8"/>
       <c r="BR60" s="8"/>
       <c r="BS60" s="8"/>
@@ -39536,13 +40192,33 @@
       <c r="BG61" s="8"/>
       <c r="BH61" s="8"/>
       <c r="BI61" s="8"/>
-      <c r="BJ61" s="8"/>
-      <c r="BK61" s="8"/>
-      <c r="BL61" s="8"/>
-      <c r="BM61" s="8"/>
-      <c r="BN61" s="8"/>
-      <c r="BO61" s="8"/>
-      <c r="BP61" s="8"/>
+      <c r="BJ61" s="16">
+        <v>23</v>
+      </c>
+      <c r="BK61" s="61" cm="1">
+        <f t="array" aca="1" ref="BK61" ca="1">BY28*$C28*$L28*POWER($F28,$O28)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A23),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL61" s="16" cm="1">
+        <f t="array" aca="1" ref="BL61" ca="1">BZ28*$C28*$L28*POWER($F28,$O28)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B23),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM61" s="16" cm="1">
+        <f t="array" aca="1" ref="BM61" ca="1">CA28*$C28*$L28*POWER($F28,$O28)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C23),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN61" s="16" cm="1">
+        <f t="array" aca="1" ref="BN61" ca="1">CB28*$C28*$L28*POWER($F28,$O28)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D23),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO61" s="16" cm="1">
+        <f t="array" aca="1" ref="BO61" ca="1">CC28*$C28*$L28*POWER($F28,$O28)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E23),9))</f>
+        <v>56</v>
+      </c>
+      <c r="BP61" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>56</v>
+      </c>
       <c r="BQ61" s="8"/>
       <c r="BR61" s="8"/>
       <c r="BS61" s="8"/>
@@ -39641,13 +40317,33 @@
       <c r="BG62" s="8"/>
       <c r="BH62" s="8"/>
       <c r="BI62" s="8"/>
-      <c r="BJ62" s="8"/>
-      <c r="BK62" s="8"/>
-      <c r="BL62" s="8"/>
-      <c r="BM62" s="8"/>
-      <c r="BN62" s="8"/>
-      <c r="BO62" s="8"/>
-      <c r="BP62" s="8"/>
+      <c r="BJ62" s="16">
+        <v>24</v>
+      </c>
+      <c r="BK62" s="61" cm="1">
+        <f t="array" aca="1" ref="BK62" ca="1">BY29*$C29*$L29*POWER($F29,$O29)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A24),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL62" s="16" cm="1">
+        <f t="array" aca="1" ref="BL62" ca="1">BZ29*$C29*$L29*POWER($F29,$O29)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B24),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM62" s="16" cm="1">
+        <f t="array" aca="1" ref="BM62" ca="1">CA29*$C29*$L29*POWER($F29,$O29)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C24),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN62" s="16" cm="1">
+        <f t="array" aca="1" ref="BN62" ca="1">CB29*$C29*$L29*POWER($F29,$O29)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D24),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BO62" s="16" cm="1">
+        <f t="array" aca="1" ref="BO62" ca="1">CC29*$C29*$L29*POWER($F29,$O29)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E24),9))</f>
+        <v>41.292619364947292</v>
+      </c>
+      <c r="BP62" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>41.292619364947292</v>
+      </c>
       <c r="BQ62" s="8"/>
       <c r="BR62" s="8"/>
       <c r="BS62" s="8"/>
@@ -39672,7 +40368,7 @@
       <c r="CL62" s="8"/>
       <c r="CM62" s="8"/>
     </row>
-    <row r="63" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:91" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A63" s="8"/>
       <c r="B63" s="7"/>
       <c r="C63" s="8">
@@ -39796,13 +40492,33 @@
       <c r="BG63" s="8"/>
       <c r="BH63" s="8"/>
       <c r="BI63" s="8"/>
-      <c r="BJ63" s="8"/>
-      <c r="BK63" s="8"/>
-      <c r="BL63" s="8"/>
-      <c r="BM63" s="8"/>
-      <c r="BN63" s="8"/>
-      <c r="BO63" s="8"/>
-      <c r="BP63" s="8"/>
+      <c r="BJ63" s="16">
+        <v>25</v>
+      </c>
+      <c r="BK63" s="61" cm="1">
+        <f t="array" aca="1" ref="BK63" ca="1">BY30*$C30*$L30*POWER($F30,$O30)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A25),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BL63" s="16" cm="1">
+        <f t="array" aca="1" ref="BL63" ca="1">BZ30*$C30*$L30*POWER($F30,$O30)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B25),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BM63" s="16" cm="1">
+        <f t="array" aca="1" ref="BM63" ca="1">CA30*$C30*$L30*POWER($F30,$O30)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C25),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BN63" s="16" cm="1">
+        <f t="array" aca="1" ref="BN63" ca="1">CB30*$C30*$L30*POWER($F30,$O30)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D25),9))</f>
+        <v>1317.3966981156575</v>
+      </c>
+      <c r="BO63" s="16" cm="1">
+        <f t="array" aca="1" ref="BO63" ca="1">CC30*$C30*$L30*POWER($F30,$O30)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E25),9))</f>
+        <v>0</v>
+      </c>
+      <c r="BP63" s="1">
+        <f t="shared" ca="1" si="23"/>
+        <v>1317.3966981156575</v>
+      </c>
       <c r="BQ63" s="8"/>
       <c r="BR63" s="8"/>
       <c r="BS63" s="8"/>
@@ -39827,11 +40543,11 @@
       <c r="CL63" s="8"/>
       <c r="CM63" s="8"/>
     </row>
-    <row r="64" spans="1:91" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:91" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A64" s="8"/>
       <c r="B64" s="7"/>
       <c r="C64" s="8">
-        <f t="shared" ref="C64:C86" si="23">SUM(AI7:AM7,AP7:AT7,AW7:BA7,BD7:BH7)</f>
+        <f t="shared" ref="C64:C86" si="24">SUM(AI7:AM7,AP7:AT7,AW7:BA7,BD7:BH7)</f>
         <v>1</v>
       </c>
       <c r="D64" s="8" t="s">
@@ -39951,14 +40667,36 @@
       <c r="BG64" s="8"/>
       <c r="BH64" s="8"/>
       <c r="BI64" s="8"/>
-      <c r="BJ64" s="8"/>
-      <c r="BK64" s="8"/>
-      <c r="BL64" s="8"/>
-      <c r="BM64" s="8"/>
-      <c r="BN64" s="8"/>
-      <c r="BO64" s="8"/>
-      <c r="BP64" s="8"/>
-      <c r="BQ64" s="8"/>
+      <c r="BJ64" s="62" t="s">
+        <v>1169</v>
+      </c>
+      <c r="BK64" s="8">
+        <f ca="1">SUM(BK39:BK63)</f>
+        <v>178.93554447148782</v>
+      </c>
+      <c r="BL64" s="8">
+        <f t="shared" ref="BL64:BO64" ca="1" si="25">SUM(BL39:BL63)</f>
+        <v>1105.5380709689553</v>
+      </c>
+      <c r="BM64" s="8">
+        <f t="shared" ca="1" si="25"/>
+        <v>3508.4675608847338</v>
+      </c>
+      <c r="BN64" s="8">
+        <f t="shared" ca="1" si="25"/>
+        <v>1800.3550364325747</v>
+      </c>
+      <c r="BO64" s="8">
+        <f t="shared" ca="1" si="25"/>
+        <v>345.052834091872</v>
+      </c>
+      <c r="BP64" s="59">
+        <f t="shared" ca="1" si="23"/>
+        <v>6938.3490468496238</v>
+      </c>
+      <c r="BQ64" s="8" t="s">
+        <v>1168</v>
+      </c>
       <c r="BR64" s="8"/>
       <c r="BS64" s="8"/>
       <c r="BT64" s="8"/>
@@ -39986,7 +40724,7 @@
       <c r="A65" s="8"/>
       <c r="B65" s="7"/>
       <c r="C65" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D65" s="8" t="s">
@@ -40141,7 +40879,7 @@
       <c r="A66" s="8"/>
       <c r="B66" s="7"/>
       <c r="C66" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D66" s="8" t="s">
@@ -40269,7 +41007,7 @@
       <c r="A67" s="8"/>
       <c r="B67" s="7"/>
       <c r="C67" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D67" s="8" t="s">
@@ -40390,7 +41128,7 @@
       <c r="A68" s="8"/>
       <c r="B68" s="10"/>
       <c r="C68" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D68" s="8" t="s">
@@ -40504,7 +41242,7 @@
       <c r="A69" s="8"/>
       <c r="B69" s="10"/>
       <c r="C69" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D69" s="8" t="s">
@@ -40618,7 +41356,7 @@
       <c r="A70" s="8"/>
       <c r="B70" s="10"/>
       <c r="C70" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D70" s="8" t="s">
@@ -40732,7 +41470,7 @@
       <c r="A71" s="8"/>
       <c r="B71" s="10"/>
       <c r="C71" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D71" s="8" t="s">
@@ -40846,7 +41584,7 @@
       <c r="A72" s="8"/>
       <c r="B72" s="10"/>
       <c r="C72" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D72" s="8" t="s">
@@ -40960,7 +41698,7 @@
       <c r="A73" s="8"/>
       <c r="B73" s="10"/>
       <c r="C73" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D73" s="8" t="s">
@@ -41074,7 +41812,7 @@
       <c r="A74" s="8"/>
       <c r="B74" s="10"/>
       <c r="C74" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D74" s="8" t="s">
@@ -41187,7 +41925,7 @@
     <row r="75" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B75" s="10"/>
       <c r="C75" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D75" s="8" t="s">
@@ -41300,7 +42038,7 @@
     <row r="76" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B76" s="7"/>
       <c r="C76" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D76" s="8" t="s">
@@ -41413,7 +42151,7 @@
     <row r="77" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B77" s="7"/>
       <c r="C77" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D77" s="8" t="s">
@@ -41526,7 +42264,7 @@
     <row r="78" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B78" s="7"/>
       <c r="C78" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D78" s="8" t="s">
@@ -41639,7 +42377,7 @@
     <row r="79" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B79" s="7"/>
       <c r="C79" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D79" s="8" t="s">
@@ -41752,7 +42490,7 @@
     <row r="80" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B80" s="7"/>
       <c r="C80" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D80" s="8" t="s">
@@ -41865,7 +42603,7 @@
     <row r="81" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B81" s="7"/>
       <c r="C81" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D81" s="8" t="s">
@@ -41978,7 +42716,7 @@
     <row r="82" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B82" s="7"/>
       <c r="C82" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>0</v>
       </c>
       <c r="D82" s="8" t="s">
@@ -42091,7 +42829,7 @@
     <row r="83" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B83" s="7"/>
       <c r="C83" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D83" s="8" t="s">
@@ -42204,7 +42942,7 @@
     <row r="84" spans="1:91" x14ac:dyDescent="0.3">
       <c r="B84" s="7"/>
       <c r="C84" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D84" s="8" t="s">
@@ -42318,7 +43056,7 @@
       <c r="A85" s="8"/>
       <c r="B85" s="7"/>
       <c r="C85" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D85" s="8" t="s">
@@ -42432,7 +43170,7 @@
       <c r="A86" s="8"/>
       <c r="B86" s="7"/>
       <c r="C86" s="8">
-        <f t="shared" si="23"/>
+        <f t="shared" si="24"/>
         <v>1</v>
       </c>
       <c r="D86" s="8" t="s">
@@ -44660,6 +45398,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100ED75AE9ACD61DF4581E288D29AF79FA4" ma:contentTypeVersion="2" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6fff2b9b3e9c3ef2196d5eeadb3d3d87">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="b79073fe-1e48-4a97-9229-baaa8603d156" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="5b8355e74ffe6f2b4bc219cfa7e75ee0" ns3:_="">
     <xsd:import namespace="b79073fe-1e48-4a97-9229-baaa8603d156"/>
@@ -44791,15 +45538,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -44807,6 +45545,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7F82F3A-971A-4E00-BEE7-5E3A8CB8E835}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7743BDCF-CD65-459D-B3C1-842DFFE4DC1D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -44824,26 +45570,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7F82F3A-971A-4E00-BEE7-5E3A8CB8E835}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9105EF9-87DC-400D-AF3A-CEFE01235C70}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="b79073fe-1e48-4a97-9229-baaa8603d156"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
excel file tolarance fixed
It was 5 in its default form now its 0
</commit_message>
<xml_diff>
--- a/IE407-Q2-v2.xlsx
+++ b/IE407-Q2-v2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://1028f8d26f624cd18d39-my.sharepoint.com/personal/e246801_metu_edu_tr/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eheng\OneDrive\Documents\GitHub\IE407-Term-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B59F4456-D29F-458E-B915-92BC2D626BA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E39AEA94-B783-4CAB-862D-311534DF6A43}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{29C75357-6D86-4F34-87D3-5ABA805A4EC9}"/>
+    <workbookView xWindow="1536" yWindow="1536" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{29C75357-6D86-4F34-87D3-5ABA805A4EC9}"/>
   </bookViews>
   <sheets>
     <sheet name="Sayfa1 Sensitivity" sheetId="2" r:id="rId1"/>
@@ -40,6 +40,7 @@
     <definedName name="solver_num" localSheetId="1" hidden="1">10</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">Sayfa1!$B$55</definedName>
+    <definedName name="solver_pre" localSheetId="1" hidden="1">0.000001</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_rel10" localSheetId="1" hidden="1">5</definedName>
     <definedName name="solver_rel2" localSheetId="1" hidden="1">3</definedName>
@@ -64,7 +65,7 @@
     <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_tol" localSheetId="1" hidden="1">0.05</definedName>
+    <definedName name="solver_tol" localSheetId="1" hidden="1">0</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">1</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
   </definedNames>
@@ -4168,10 +4169,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="40" name="OpenSolver1">
+        <xdr:cNvPr id="116" name="OpenSolver1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F71AF40D-C38D-4E1B-BC05-5FB74E9AC844}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{57EABE5E-F67C-427B-8C26-FB743A1D4BC5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4256,10 +4257,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="41" name="OpenSolver2">
+        <xdr:cNvPr id="117" name="OpenSolver2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{667D5C69-43F7-47CE-854F-45FCEB357439}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{70A0A76B-2053-4CFC-93CA-58D8E6E67829}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4344,10 +4345,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="42" name="OpenSolver3">
+        <xdr:cNvPr id="118" name="OpenSolver3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{2968F20C-E26D-43A1-A8D7-D657276497EA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1E5A1422-60DE-4C22-A860-2E98565FF365}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4432,10 +4433,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="43" name="OpenSolver4">
+        <xdr:cNvPr id="119" name="OpenSolver4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{66651AEE-1500-4269-AF8A-1753BF902079}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D85E3722-A028-45B0-ACCD-9787D5CDBAC0}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4520,10 +4521,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="44" name="OpenSolver5">
+        <xdr:cNvPr id="120" name="OpenSolver5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A36E8F17-8786-401A-A6FA-C6BA91CE9267}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{AA36B616-5F45-468D-8B3B-150855E37F27}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4602,10 +4603,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="45" name="OpenSolver6">
+        <xdr:cNvPr id="121" name="OpenSolver6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BB6317E0-F7A5-46C9-A5C5-08A2541A1BCC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{842898C0-41BE-440F-95E9-847007B68EF3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4691,14 +4692,14 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="46" name="OpenSolver7">
+        <xdr:cNvPr id="122" name="OpenSolver7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6986BD4F-25E9-484D-ABBF-EFBAA1B5C31E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6D040DE-1D8C-4A86-90DD-F069C20233CC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4707,7 +4708,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="1485900" y="12329160"/>
-          <a:ext cx="754380" cy="4953001"/>
+          <a:ext cx="754380" cy="4968240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4773,14 +4774,14 @@
       <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="47" name="OpenSolver8">
+        <xdr:cNvPr id="123" name="OpenSolver8">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9FDA1227-529A-4CFC-985B-24FBD3BA5932}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3FF2B8AB-DEA8-49C2-88EF-833E6DBBDDDD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4789,7 +4790,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="3108960" y="12329160"/>
-          <a:ext cx="617220" cy="4953001"/>
+          <a:ext cx="617220" cy="4968240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -4852,31 +4853,31 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="48" name="OpenSolver9">
+        <xdr:cNvPr id="124" name="OpenSolver9">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B55DE01-2D26-42F9-9B4B-7F9571F321A4}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6C160358-BE09-4677-B5F0-C58D5C8C7BD2}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="46" idx="3"/>
-          <a:endCxn id="47" idx="1"/>
+          <a:stCxn id="122" idx="3"/>
+          <a:endCxn id="123" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2240280" y="14805661"/>
+          <a:off x="2240280" y="14813280"/>
           <a:ext cx="868680" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -4913,20 +4914,20 @@
       <xdr:col>3</xdr:col>
       <xdr:colOff>243840</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>170181</xdr:rowOff>
+      <xdr:rowOff>162560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>624840</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>27941</xdr:rowOff>
+      <xdr:rowOff>20320</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="49" name="OpenSolver10">
+        <xdr:cNvPr id="125" name="OpenSolver10">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{32A459F0-EB74-4F3C-85E9-774041A8838C}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B3283237-4E18-4B31-988D-1883C39FC105}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -4934,7 +4935,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="2484120" y="14678661"/>
+          <a:off x="2484120" y="14686280"/>
           <a:ext cx="381000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5006,14 +5007,14 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="50" name="OpenSolver11">
+        <xdr:cNvPr id="126" name="OpenSolver11">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6383258A-88E2-458D-9C08-CF604E47E79E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{20484480-4D30-4251-9EDB-114BE4A9EA56}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5022,7 +5023,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="5105400" y="12329160"/>
-          <a:ext cx="617220" cy="4953001"/>
+          <a:ext cx="617220" cy="4968240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5088,14 +5089,14 @@
       <xdr:col>10</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="51" name="OpenSolver12">
+        <xdr:cNvPr id="127" name="OpenSolver12">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE6DFFDF-4DCD-4102-8934-154DE933088B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{45A199A9-2E10-4E1E-A06A-12CA572C03E3}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5104,7 +5105,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="6553200" y="12329160"/>
-          <a:ext cx="617220" cy="4953001"/>
+          <a:ext cx="617220" cy="4968240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5167,31 +5168,31 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="52" name="OpenSolver13">
+        <xdr:cNvPr id="128" name="OpenSolver13">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BA74D4C7-9381-47D6-A532-17D9315753E6}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3B19728B-5717-4A2A-8225-A150B20C10BD}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="50" idx="3"/>
-          <a:endCxn id="51" idx="1"/>
+          <a:stCxn id="126" idx="3"/>
+          <a:endCxn id="127" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5722620" y="14805661"/>
+          <a:off x="5722620" y="14813280"/>
           <a:ext cx="830580" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -5228,20 +5229,20 @@
       <xdr:col>8</xdr:col>
       <xdr:colOff>224790</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>170181</xdr:rowOff>
+      <xdr:rowOff>162560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
       <xdr:colOff>605790</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>27941</xdr:rowOff>
+      <xdr:rowOff>20320</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="53" name="OpenSolver14">
+        <xdr:cNvPr id="129" name="OpenSolver14">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D1BF2760-7A9F-46B5-8203-C7AD0CB3692A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{526819B7-D602-43A6-A018-36AD7BCF58B1}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5249,7 +5250,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5947410" y="14678661"/>
+          <a:off x="5947410" y="14686280"/>
           <a:ext cx="381000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5321,14 +5322,14 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="54" name="OpenSolver15">
+        <xdr:cNvPr id="130" name="OpenSolver15">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8A992895-244B-4807-8252-01C2A8886D85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4040F08-CFE8-453A-8464-9CA15A6917CB}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5337,7 +5338,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="8404860" y="12329160"/>
-          <a:ext cx="617220" cy="4953001"/>
+          <a:ext cx="617220" cy="4968240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5403,14 +5404,14 @@
       <xdr:col>15</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>87</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="55" name="OpenSolver16">
+        <xdr:cNvPr id="131" name="OpenSolver16">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EF8A67CD-E442-461B-9759-C2A88853F295}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E26A544E-B8CB-4AB0-B8BC-FC3AACE6DA6A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5419,7 +5420,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="9639300" y="12329160"/>
-          <a:ext cx="617220" cy="4953001"/>
+          <a:ext cx="617220" cy="4968240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5482,31 +5483,31 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>74</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="56" name="OpenSolver17">
+        <xdr:cNvPr id="132" name="OpenSolver17">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5CC932A7-1F42-44B2-8772-3A7D714DFF56}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DB9F0528-F23C-4230-8745-C079A1D5077D}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="54" idx="3"/>
-          <a:endCxn id="55" idx="1"/>
+          <a:stCxn id="130" idx="3"/>
+          <a:endCxn id="131" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9022080" y="14805661"/>
+          <a:off x="9022080" y="14813280"/>
           <a:ext cx="617220" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -5543,20 +5544,20 @@
       <xdr:col>13</xdr:col>
       <xdr:colOff>118110</xdr:colOff>
       <xdr:row>73</xdr:row>
-      <xdr:rowOff>170181</xdr:rowOff>
+      <xdr:rowOff>162560</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
       <xdr:colOff>499110</xdr:colOff>
       <xdr:row>75</xdr:row>
-      <xdr:rowOff>27941</xdr:rowOff>
+      <xdr:rowOff>20320</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="57" name="OpenSolver18">
+        <xdr:cNvPr id="133" name="OpenSolver18">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{21878EA8-4CDC-4DC7-B862-12C9BA0BD059}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{122E5712-9D30-4B3F-AE85-C650CEFF8B2B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5564,7 +5565,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9140190" y="14678661"/>
+          <a:off x="9140190" y="14686280"/>
           <a:ext cx="381000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5636,14 +5637,14 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>617219</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="58" name="OpenSolver19">
+        <xdr:cNvPr id="134" name="OpenSolver19">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FA887D8F-62D9-4AE9-BE79-C3467B26CD65}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5E32359D-FB37-423B-A4F5-E1343A47B7F6}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5652,7 +5653,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="11551920" y="12329160"/>
-          <a:ext cx="617219" cy="990601"/>
+          <a:ext cx="617219" cy="1005840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5718,14 +5719,14 @@
       <xdr:col>20</xdr:col>
       <xdr:colOff>1</xdr:colOff>
       <xdr:row>67</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="59" name="OpenSolver20">
+        <xdr:cNvPr id="135" name="OpenSolver20">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DE082AA7-8D5C-45F9-853C-8196DF2DCC51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D2ABE7B7-0876-4643-80D8-1E0A0D635241}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5734,7 +5735,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12778740" y="12329160"/>
-          <a:ext cx="617221" cy="990601"/>
+          <a:ext cx="617221" cy="1005840"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -5797,31 +5798,31 @@
       <xdr:col>17</xdr:col>
       <xdr:colOff>617219</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>99061</xdr:rowOff>
+      <xdr:rowOff>91440</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="60" name="OpenSolver21">
+        <xdr:cNvPr id="136" name="OpenSolver21">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FAA25DA6-32D5-48F8-A068-AAF0522D71F8}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1C83DE93-F81D-43F8-9854-7F507BCF65D5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="58" idx="3"/>
-          <a:endCxn id="59" idx="1"/>
+          <a:stCxn id="134" idx="3"/>
+          <a:endCxn id="135" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12169139" y="12824461"/>
+          <a:off x="12169139" y="12832080"/>
           <a:ext cx="609601" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -5858,20 +5859,20 @@
       <xdr:col>18</xdr:col>
       <xdr:colOff>114300</xdr:colOff>
       <xdr:row>63</xdr:row>
-      <xdr:rowOff>170181</xdr:rowOff>
+      <xdr:rowOff>170180</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>18</xdr:col>
       <xdr:colOff>495300</xdr:colOff>
       <xdr:row>65</xdr:row>
-      <xdr:rowOff>27941</xdr:rowOff>
+      <xdr:rowOff>20320</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="61" name="OpenSolver22">
+        <xdr:cNvPr id="137" name="OpenSolver22">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FC6EF0B8-A0F4-415F-BAE1-6CC58E8C9F91}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F76A101C-BD0C-413F-BFC7-BB805D843F98}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5879,7 +5880,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="12283440" y="12697461"/>
+          <a:off x="12283440" y="12705080"/>
           <a:ext cx="381000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -5950,15 +5951,15 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>198119</xdr:rowOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="62" name="OpenSolver23">
+        <xdr:cNvPr id="138" name="OpenSolver23">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C369C158-BA79-437F-B0D5-7746A568A04B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D878E15E-D87E-49FA-872E-C00369BF8F0A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -5967,7 +5968,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="14622780" y="12329160"/>
-          <a:ext cx="617220" cy="792479"/>
+          <a:ext cx="617220" cy="807720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6032,15 +6033,15 @@
     <xdr:to>
       <xdr:col>25</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>65</xdr:row>
-      <xdr:rowOff>198119</xdr:rowOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="63" name="OpenSolver24">
+        <xdr:cNvPr id="139" name="OpenSolver24">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B106CC3-CE5A-4713-8647-476AD757273E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{911CFE64-80BA-40D4-B32C-BB7EF2D6BF7E}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6049,7 +6050,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="15925800" y="12329160"/>
-          <a:ext cx="617220" cy="792479"/>
+          <a:ext cx="617220" cy="807720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6111,32 +6112,32 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>198120</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>198120</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="64" name="OpenSolver25">
+        <xdr:cNvPr id="140" name="OpenSolver25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{95681D30-6657-4FB2-AEBF-BDFC09770C85}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{59A316AC-21DB-426A-93C5-B990A6FBE1B7}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="62" idx="3"/>
-          <a:endCxn id="63" idx="1"/>
+          <a:stCxn id="138" idx="3"/>
+          <a:endCxn id="139" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15240000" y="12725400"/>
+          <a:off x="15240000" y="12733020"/>
           <a:ext cx="685800" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -6179,14 +6180,14 @@
       <xdr:col>23</xdr:col>
       <xdr:colOff>533400</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>127000</xdr:rowOff>
+      <xdr:rowOff>119380</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="65" name="OpenSolver26">
+        <xdr:cNvPr id="141" name="OpenSolver26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{99ED5F60-C731-4BC3-B279-DF4F089511DD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3264406F-606B-4D9F-9A0B-A160963AAE87}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6194,7 +6195,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="15392400" y="12598400"/>
+          <a:off x="15392400" y="12606020"/>
           <a:ext cx="381000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6270,10 +6271,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="66" name="OpenSolver27">
+        <xdr:cNvPr id="142" name="OpenSolver27">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{42045BA8-DB7B-48A1-AA6D-A09E8C17FC51}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{284D1BCD-9E95-4CAC-A3FF-C0E2882A0E3C}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6282,7 +6283,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="17777461" y="12329160"/>
-          <a:ext cx="3131819" cy="594360"/>
+          <a:ext cx="3131819" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6352,10 +6353,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="67" name="OpenSolver28">
+        <xdr:cNvPr id="143" name="OpenSolver28">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F1B1CD39-6E2E-4A53-8EC3-1D58940646A7}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{326AFAC7-063F-4176-BD11-EC59CB7EC0BF}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6364,7 +6365,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="21526500" y="12329160"/>
-          <a:ext cx="3322320" cy="594360"/>
+          <a:ext cx="3322320" cy="609600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -6437,21 +6438,21 @@
     </xdr:to>
     <xdr:cxnSp macro="">
       <xdr:nvCxnSpPr>
-        <xdr:cNvPr id="68" name="OpenSolver29">
+        <xdr:cNvPr id="144" name="OpenSolver29">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A4E44D99-74F7-4063-A565-3A480442C770}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3408EDC3-7B30-45DE-9DD1-5F23BA92CD71}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
         <xdr:cNvCxnSpPr>
-          <a:stCxn id="66" idx="3"/>
-          <a:endCxn id="67" idx="1"/>
+          <a:stCxn id="142" idx="3"/>
+          <a:endCxn id="143" idx="1"/>
         </xdr:cNvCxnSpPr>
       </xdr:nvCxnSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="20909280" y="12626340"/>
+          <a:off x="20909280" y="12633960"/>
           <a:ext cx="617220" cy="0"/>
         </a:xfrm>
         <a:prstGeom prst="straightConnector1">
@@ -6488,20 +6489,20 @@
       <xdr:col>32</xdr:col>
       <xdr:colOff>118111</xdr:colOff>
       <xdr:row>62</xdr:row>
-      <xdr:rowOff>170180</xdr:rowOff>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>32</xdr:col>
       <xdr:colOff>499111</xdr:colOff>
       <xdr:row>64</xdr:row>
-      <xdr:rowOff>27940</xdr:rowOff>
+      <xdr:rowOff>20320</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="69" name="OpenSolver30">
+        <xdr:cNvPr id="145" name="OpenSolver30">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{645165AD-02BF-4CFB-BC02-4DD68CBF793B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{CFB0580B-8E7E-42B9-B101-07A9CB94C433}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6509,7 +6510,7 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="21027391" y="12499340"/>
+          <a:off x="21027391" y="12506960"/>
           <a:ext cx="381000" cy="254000"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -6585,10 +6586,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="70" name="OpenSolver31">
+        <xdr:cNvPr id="146" name="OpenSolver31">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53E937B6-B3EE-4857-ABAE-E4B28536479B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B055900D-6F99-4BEF-92A2-033890715139}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6667,10 +6668,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="71" name="OpenSolver32">
+        <xdr:cNvPr id="147" name="OpenSolver32">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4672B8E0-170D-4F61-929A-02874B1B0B64}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9E6249E4-3553-4CA0-99C8-0E029891818B}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6760,10 +6761,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="72" name="OpenSolver33">
+        <xdr:cNvPr id="148" name="OpenSolver33">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{48E9FAB7-5B97-484C-B30F-67834FBC8B4E}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED08C0DA-1364-477A-ADA1-72DB90CF6574}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6842,10 +6843,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="73" name="OpenSolver34">
+        <xdr:cNvPr id="149" name="OpenSolver34">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3D4FA2AA-BA98-4368-BF34-F96088B014C1}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D29AF873-25A8-4EA4-B586-57CD65F0E6E5}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -6935,10 +6936,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="74" name="OpenSolver35">
+        <xdr:cNvPr id="150" name="OpenSolver35">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FDCEC243-56E8-4221-A7CF-A1463C65E07B}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DD2F9906-84B8-479E-8455-6A94D1CD31A4}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7017,10 +7018,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="75" name="OpenSolver36">
+        <xdr:cNvPr id="151" name="OpenSolver36">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4F080CB5-4934-4356-9BA9-CAC593587009}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DBC2F5A1-5E72-4C17-A7AA-E0E18AE9B103}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7110,10 +7111,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="76" name="OpenSolver37">
+        <xdr:cNvPr id="152" name="OpenSolver37">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{382F5A23-0D2D-4047-91B5-A4D998750FBD}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D4174AA3-FE64-4194-B1CE-E72A6C9DB652}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -7192,10 +7193,10 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="77" name="OpenSolver38">
+        <xdr:cNvPr id="153" name="OpenSolver38">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0B79BA49-10D5-4550-B434-C930C7417FB3}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8C69F414-0D08-4041-8DC6-FD04C4FC7409}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -32001,8 +32002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7930316F-CD20-49E5-A6A0-4C42FB60CBBA}">
   <dimension ref="A1:CM132"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="BQ57" sqref="BQ57"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K51" sqref="K51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -33286,13 +33287,13 @@
         <v>0</v>
       </c>
       <c r="AK9" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL9" s="16">
         <v>0</v>
       </c>
       <c r="AM9" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN9" s="8"/>
       <c r="AO9" s="23">
@@ -33364,7 +33365,7 @@
       </c>
       <c r="BM9" s="16">
         <f t="shared" si="10"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BN9" s="16">
         <f t="shared" si="11"/>
@@ -33372,7 +33373,7 @@
       </c>
       <c r="BO9" s="16">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP9" s="8"/>
       <c r="BQ9" s="23">
@@ -33388,7 +33389,7 @@
       </c>
       <c r="BT9" s="16">
         <f t="shared" si="15"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BU9" s="16">
         <f t="shared" si="16"/>
@@ -33396,7 +33397,7 @@
       </c>
       <c r="BV9" s="16">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW9" s="8"/>
       <c r="BX9" s="23">
@@ -33412,7 +33413,7 @@
       </c>
       <c r="CA9" s="16">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="CB9" s="16">
         <f t="shared" si="21"/>
@@ -33420,7 +33421,7 @@
       </c>
       <c r="CC9" s="19">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="10" spans="2:81" x14ac:dyDescent="0.3">
@@ -33740,7 +33741,7 @@
         <v>0</v>
       </c>
       <c r="AM11" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN11" s="8"/>
       <c r="AO11" s="23">
@@ -33820,7 +33821,7 @@
       </c>
       <c r="BO11" s="16">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP11" s="8"/>
       <c r="BQ11" s="23">
@@ -33844,7 +33845,7 @@
       </c>
       <c r="BV11" s="16">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW11" s="8"/>
       <c r="BX11" s="23">
@@ -33868,7 +33869,7 @@
       </c>
       <c r="CC11" s="19">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="2:81" x14ac:dyDescent="0.3">
@@ -34176,7 +34177,7 @@
         <v>8</v>
       </c>
       <c r="AI13" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ13" s="16">
         <v>0</v>
@@ -34188,7 +34189,7 @@
         <v>0</v>
       </c>
       <c r="AM13" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN13" s="8"/>
       <c r="AO13" s="23">
@@ -34252,7 +34253,7 @@
       </c>
       <c r="BK13" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL13" s="16">
         <f t="shared" si="9"/>
@@ -34268,7 +34269,7 @@
       </c>
       <c r="BO13" s="16">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP13" s="8"/>
       <c r="BQ13" s="23">
@@ -34276,7 +34277,7 @@
       </c>
       <c r="BR13" s="16">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS13" s="16">
         <f t="shared" si="14"/>
@@ -34292,7 +34293,7 @@
       </c>
       <c r="BV13" s="16">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BW13" s="8"/>
       <c r="BX13" s="23">
@@ -34300,7 +34301,7 @@
       </c>
       <c r="BY13" s="16">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ13" s="16">
         <f t="shared" si="19"/>
@@ -34316,7 +34317,7 @@
       </c>
       <c r="CC13" s="19">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:81" x14ac:dyDescent="0.3">
@@ -34441,13 +34442,13 @@
         <v>0</v>
       </c>
       <c r="AX14" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AY14" s="16">
         <v>0</v>
       </c>
       <c r="AZ14" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BA14" s="16">
         <v>0</v>
@@ -34480,7 +34481,7 @@
       </c>
       <c r="BL14" s="16">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM14" s="16">
         <f t="shared" si="10"/>
@@ -34488,7 +34489,7 @@
       </c>
       <c r="BN14" s="16">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO14" s="16">
         <f t="shared" si="12"/>
@@ -34504,7 +34505,7 @@
       </c>
       <c r="BS14" s="16">
         <f t="shared" si="14"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BT14" s="16">
         <f t="shared" si="15"/>
@@ -34512,7 +34513,7 @@
       </c>
       <c r="BU14" s="16">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BV14" s="16">
         <f t="shared" si="17"/>
@@ -34528,7 +34529,7 @@
       </c>
       <c r="BZ14" s="16">
         <f t="shared" si="19"/>
-        <v>2.4082246852806923</v>
+        <v>0</v>
       </c>
       <c r="CA14" s="16">
         <f t="shared" si="20"/>
@@ -34536,7 +34537,7 @@
       </c>
       <c r="CB14" s="16">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>2.4082246852806923</v>
       </c>
       <c r="CC14" s="19">
         <f t="shared" si="22"/>
@@ -34662,7 +34663,7 @@
         <v>10</v>
       </c>
       <c r="AW15" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AX15" s="16">
         <v>0</v>
@@ -34674,7 +34675,7 @@
         <v>0</v>
       </c>
       <c r="BA15" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BB15" s="8"/>
       <c r="BC15" s="23">
@@ -34700,7 +34701,7 @@
       </c>
       <c r="BK15" s="16">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL15" s="16">
         <f t="shared" si="9"/>
@@ -34716,7 +34717,7 @@
       </c>
       <c r="BO15" s="16">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP15" s="8"/>
       <c r="BQ15" s="23">
@@ -34724,7 +34725,7 @@
       </c>
       <c r="BR15" s="16">
         <f t="shared" si="13"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BS15" s="16">
         <f t="shared" si="14"/>
@@ -34740,7 +34741,7 @@
       </c>
       <c r="BV15" s="16">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="BW15" s="8"/>
       <c r="BX15" s="23">
@@ -34748,7 +34749,7 @@
       </c>
       <c r="BY15" s="16">
         <f t="shared" si="18"/>
-        <v>2.4082246852806923</v>
+        <v>0</v>
       </c>
       <c r="BZ15" s="16">
         <f t="shared" si="19"/>
@@ -34764,7 +34765,7 @@
       </c>
       <c r="CC15" s="19">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>2.4082246852806923</v>
       </c>
     </row>
     <row r="16" spans="2:81" x14ac:dyDescent="0.3">
@@ -34848,13 +34849,13 @@
         <v>11</v>
       </c>
       <c r="AI16" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ16" s="16">
         <v>0</v>
       </c>
       <c r="AK16" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AL16" s="16">
         <v>0</v>
@@ -34924,7 +34925,7 @@
       </c>
       <c r="BK16" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL16" s="16">
         <f t="shared" si="9"/>
@@ -34932,7 +34933,7 @@
       </c>
       <c r="BM16" s="16">
         <f t="shared" si="10"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BN16" s="16">
         <f t="shared" si="11"/>
@@ -34948,7 +34949,7 @@
       </c>
       <c r="BR16" s="16">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BS16" s="16">
         <f t="shared" si="14"/>
@@ -34956,7 +34957,7 @@
       </c>
       <c r="BT16" s="16">
         <f t="shared" si="15"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BU16" s="16">
         <f t="shared" si="16"/>
@@ -34972,7 +34973,7 @@
       </c>
       <c r="BY16" s="16">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BZ16" s="16">
         <f t="shared" si="19"/>
@@ -34980,7 +34981,7 @@
       </c>
       <c r="CA16" s="16">
         <f t="shared" si="20"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="CB16" s="16">
         <f t="shared" si="21"/>
@@ -35804,13 +35805,13 @@
         <v>0</v>
       </c>
       <c r="BE20" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BF20" s="16">
         <v>0</v>
       </c>
       <c r="BG20" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BH20" s="19">
         <v>0</v>
@@ -35824,7 +35825,7 @@
       </c>
       <c r="BL20" s="16">
         <f t="shared" si="9"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BM20" s="16">
         <f t="shared" si="10"/>
@@ -35832,7 +35833,7 @@
       </c>
       <c r="BN20" s="16">
         <f t="shared" si="11"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BO20" s="16">
         <f t="shared" si="12"/>
@@ -35848,7 +35849,7 @@
       </c>
       <c r="BS20" s="16">
         <f t="shared" si="14"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BT20" s="16">
         <f t="shared" si="15"/>
@@ -35856,7 +35857,7 @@
       </c>
       <c r="BU20" s="16">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BV20" s="16">
         <f t="shared" si="17"/>
@@ -35872,7 +35873,7 @@
       </c>
       <c r="BZ20" s="16">
         <f t="shared" si="19"/>
-        <v>3.031433133020796</v>
+        <v>0</v>
       </c>
       <c r="CA20" s="16">
         <f t="shared" si="20"/>
@@ -35880,7 +35881,7 @@
       </c>
       <c r="CB20" s="16">
         <f t="shared" si="21"/>
-        <v>0</v>
+        <v>3.031433133020796</v>
       </c>
       <c r="CC20" s="19">
         <f t="shared" si="22"/>
@@ -37107,7 +37108,7 @@
         <v>21</v>
       </c>
       <c r="AP26" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AQ26" s="16">
         <v>0</v>
@@ -37138,7 +37139,7 @@
         <v>0</v>
       </c>
       <c r="BA26" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BB26" s="8"/>
       <c r="BC26" s="23">
@@ -37164,7 +37165,7 @@
       </c>
       <c r="BK26" s="16">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BL26" s="16">
         <f t="shared" si="9"/>
@@ -37180,7 +37181,7 @@
       </c>
       <c r="BO26" s="16">
         <f t="shared" si="12"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BP26" s="8"/>
       <c r="BQ26" s="23">
@@ -37188,7 +37189,7 @@
       </c>
       <c r="BR26" s="16">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="BS26" s="16">
         <f t="shared" si="14"/>
@@ -37204,7 +37205,7 @@
       </c>
       <c r="BV26" s="16">
         <f t="shared" si="17"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="BW26" s="8"/>
       <c r="BX26" s="23">
@@ -37212,7 +37213,7 @@
       </c>
       <c r="BY26" s="16">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1.515716566510398</v>
       </c>
       <c r="BZ26" s="16">
         <f t="shared" si="19"/>
@@ -37228,7 +37229,7 @@
       </c>
       <c r="CC26" s="19">
         <f t="shared" si="22"/>
-        <v>1.9331820449317627</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="2:81" x14ac:dyDescent="0.3">
@@ -37312,7 +37313,7 @@
         <v>22</v>
       </c>
       <c r="AI27" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AJ27" s="16">
         <v>0</v>
@@ -37324,7 +37325,7 @@
         <v>0</v>
       </c>
       <c r="AM27" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN27" s="8"/>
       <c r="AO27" s="23">
@@ -37388,7 +37389,7 @@
       </c>
       <c r="BK27" s="16">
         <f t="shared" si="8"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BL27" s="16">
         <f t="shared" si="9"/>
@@ -37404,7 +37405,7 @@
       </c>
       <c r="BO27" s="16">
         <f t="shared" si="12"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BP27" s="8"/>
       <c r="BQ27" s="23">
@@ -37412,7 +37413,7 @@
       </c>
       <c r="BR27" s="16">
         <f t="shared" si="13"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BS27" s="16">
         <f t="shared" si="14"/>
@@ -37428,7 +37429,7 @@
       </c>
       <c r="BV27" s="16">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BW27" s="8"/>
       <c r="BX27" s="23">
@@ -37436,7 +37437,7 @@
       </c>
       <c r="BY27" s="16">
         <f t="shared" si="18"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BZ27" s="16">
         <f t="shared" si="19"/>
@@ -37452,7 +37453,7 @@
       </c>
       <c r="CC27" s="19">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="28" spans="2:81" x14ac:dyDescent="0.3">
@@ -37772,7 +37773,7 @@
         <v>0</v>
       </c>
       <c r="AM29" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AN29" s="8"/>
       <c r="AO29" s="23">
@@ -37791,7 +37792,7 @@
         <v>0</v>
       </c>
       <c r="AT29" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AU29" s="8"/>
       <c r="AV29" s="23">
@@ -37876,7 +37877,7 @@
       </c>
       <c r="BV29" s="16">
         <f t="shared" si="17"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="BW29" s="8"/>
       <c r="BX29" s="23">
@@ -37900,7 +37901,7 @@
       </c>
       <c r="CC29" s="19">
         <f t="shared" si="22"/>
-        <v>1</v>
+        <v>1.7411011265922482</v>
       </c>
     </row>
     <row r="30" spans="2:81" x14ac:dyDescent="0.3">
@@ -38044,13 +38045,13 @@
         <v>0</v>
       </c>
       <c r="BE30" s="16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BF30" s="16">
         <v>0</v>
       </c>
       <c r="BG30" s="16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BH30" s="19">
         <v>0</v>
@@ -38064,7 +38065,7 @@
       </c>
       <c r="BL30" s="16">
         <f t="shared" si="9"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="BM30" s="16">
         <f t="shared" si="10"/>
@@ -38072,7 +38073,7 @@
       </c>
       <c r="BN30" s="16">
         <f t="shared" si="11"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="BO30" s="16">
         <f t="shared" si="12"/>
@@ -38088,7 +38089,7 @@
       </c>
       <c r="BS30" s="16">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="BT30" s="16">
         <f t="shared" si="15"/>
@@ -38096,7 +38097,7 @@
       </c>
       <c r="BU30" s="16">
         <f t="shared" si="16"/>
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="BV30" s="16">
         <f t="shared" si="17"/>
@@ -38112,7 +38113,7 @@
       </c>
       <c r="BZ30" s="16">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>3.4822022531844965</v>
       </c>
       <c r="CA30" s="16">
         <f t="shared" si="20"/>
@@ -38120,7 +38121,7 @@
       </c>
       <c r="CB30" s="16">
         <f t="shared" si="21"/>
-        <v>3.4822022531844965</v>
+        <v>0</v>
       </c>
       <c r="CC30" s="19">
         <f t="shared" si="22"/>
@@ -38916,7 +38917,7 @@
       </c>
       <c r="BM42" s="16" cm="1">
         <f t="array" aca="1" ref="BM42" ca="1">CA9*$C9*$L9*POWER($F9,$O9)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C4),9))</f>
-        <v>0</v>
+        <v>61.982472786971179</v>
       </c>
       <c r="BN42" s="16" cm="1">
         <f t="array" aca="1" ref="BN42" ca="1">CB9*$C9*$L9*POWER($F9,$O9)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D4),9))</f>
@@ -38924,11 +38925,11 @@
       </c>
       <c r="BO42" s="16" cm="1">
         <f t="array" aca="1" ref="BO42" ca="1">CC9*$C9*$L9*POWER($F9,$O9)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E4),9))</f>
-        <v>15.495618196742795</v>
+        <v>0</v>
       </c>
       <c r="BP42" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>15.495618196742795</v>
+        <v>61.982472786971179</v>
       </c>
     </row>
     <row r="43" spans="2:81" x14ac:dyDescent="0.3">
@@ -39052,11 +39053,11 @@
       </c>
       <c r="BO44" s="16" cm="1">
         <f t="array" aca="1" ref="BO44" ca="1">CC11*$C11*$L11*POWER($F11,$O11)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E6),9))</f>
-        <v>0</v>
+        <v>14.333707577554534</v>
       </c>
       <c r="BP44" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>0</v>
+        <v>14.333707577554534</v>
       </c>
     </row>
     <row r="45" spans="2:81" x14ac:dyDescent="0.3">
@@ -39158,7 +39159,7 @@
       </c>
       <c r="BK46" s="61" cm="1">
         <f t="array" aca="1" ref="BK46" ca="1">BY13*$C13*$L13*POWER($F13,$O13)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A8),9))</f>
-        <v>0</v>
+        <v>14.585909370234862</v>
       </c>
       <c r="BL46" s="16" cm="1">
         <f t="array" aca="1" ref="BL46" ca="1">BZ13*$C13*$L13*POWER($F13,$O13)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B8),9))</f>
@@ -39174,7 +39175,7 @@
       </c>
       <c r="BO46" s="16" cm="1">
         <f t="array" aca="1" ref="BO46" ca="1">CC13*$C13*$L13*POWER($F13,$O13)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E8),9))</f>
-        <v>14.585909370234862</v>
+        <v>0</v>
       </c>
       <c r="BP46" s="1">
         <f t="shared" ca="1" si="23"/>
@@ -39226,7 +39227,7 @@
       </c>
       <c r="BL47" s="16" cm="1">
         <f t="array" aca="1" ref="BL47" ca="1">BZ14*$C14*$L14*POWER($F14,$O14)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B9),9))</f>
-        <v>293.2988134700031</v>
+        <v>0</v>
       </c>
       <c r="BM47" s="16" cm="1">
         <f t="array" aca="1" ref="BM47" ca="1">CA14*$C14*$L14*POWER($F14,$O14)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C9),9))</f>
@@ -39234,7 +39235,7 @@
       </c>
       <c r="BN47" s="16" cm="1">
         <f t="array" aca="1" ref="BN47" ca="1">CB14*$C14*$L14*POWER($F14,$O14)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D9),9))</f>
-        <v>0</v>
+        <v>293.2988134700031</v>
       </c>
       <c r="BO47" s="16" cm="1">
         <f t="array" aca="1" ref="BO47" ca="1">CC14*$C14*$L14*POWER($F14,$O14)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E9),9))</f>
@@ -39289,7 +39290,7 @@
       </c>
       <c r="BK48" s="61" cm="1">
         <f t="array" aca="1" ref="BK48" ca="1">BY15*$C15*$L15*POWER($F15,$O15)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A10),9))</f>
-        <v>125.3576818177493</v>
+        <v>0</v>
       </c>
       <c r="BL48" s="16" cm="1">
         <f t="array" aca="1" ref="BL48" ca="1">BZ15*$C15*$L15*POWER($F15,$O15)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B10),9))</f>
@@ -39305,7 +39306,7 @@
       </c>
       <c r="BO48" s="16" cm="1">
         <f t="array" aca="1" ref="BO48" ca="1">CC15*$C15*$L15*POWER($F15,$O15)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E10),9))</f>
-        <v>0</v>
+        <v>125.3576818177493</v>
       </c>
       <c r="BP48" s="1">
         <f t="shared" ca="1" si="23"/>
@@ -39357,7 +39358,7 @@
       </c>
       <c r="BK49" s="61" cm="1">
         <f t="array" aca="1" ref="BK49" ca="1">BY16*$C16*$L16*POWER($F16,$O16)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A11),9))</f>
-        <v>0</v>
+        <v>14.577768528468802</v>
       </c>
       <c r="BL49" s="16" cm="1">
         <f t="array" aca="1" ref="BL49" ca="1">BZ16*$C16*$L16*POWER($F16,$O16)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B11),9))</f>
@@ -39365,7 +39366,7 @@
       </c>
       <c r="BM49" s="16" cm="1">
         <f t="array" aca="1" ref="BM49" ca="1">CA16*$C16*$L16*POWER($F16,$O16)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C11),9))</f>
-        <v>58.311074113875208</v>
+        <v>0</v>
       </c>
       <c r="BN49" s="16" cm="1">
         <f t="array" aca="1" ref="BN49" ca="1">CB16*$C16*$L16*POWER($F16,$O16)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D11),9))</f>
@@ -39377,7 +39378,7 @@
       </c>
       <c r="BP49" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>58.311074113875208</v>
+        <v>14.577768528468802</v>
       </c>
     </row>
     <row r="50" spans="1:91" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
@@ -39550,7 +39551,7 @@
       </c>
       <c r="BL53" s="16" cm="1">
         <f t="array" aca="1" ref="BL53" ca="1">BZ20*$C20*$L20*POWER($F20,$O20)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B15),9))</f>
-        <v>812.23925749895227</v>
+        <v>0</v>
       </c>
       <c r="BM53" s="16" cm="1">
         <f t="array" aca="1" ref="BM53" ca="1">CA20*$C20*$L20*POWER($F20,$O20)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C15),9))</f>
@@ -39558,7 +39559,7 @@
       </c>
       <c r="BN53" s="16" cm="1">
         <f t="array" aca="1" ref="BN53" ca="1">CB20*$C20*$L20*POWER($F20,$O20)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D15),9))</f>
-        <v>0</v>
+        <v>812.23925749895227</v>
       </c>
       <c r="BO53" s="16" cm="1">
         <f t="array" aca="1" ref="BO53" ca="1">CC20*$C20*$L20*POWER($F20,$O20)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E15),9))</f>
@@ -39611,7 +39612,7 @@
     <row r="55" spans="1:91" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B55" s="25" cm="1">
         <f t="array" ref="B55">SUMPRODUCT(MMULT(BY6:CC30*C6:C30*L6:L30*POWER(F6:F30,O6:O30),I33:I37))</f>
-        <v>6938.3490468496238</v>
+        <v>6945.7335192189566</v>
       </c>
       <c r="C55" s="26"/>
       <c r="D55" s="26"/>
@@ -39971,7 +39972,7 @@
       </c>
       <c r="BK59" s="61" cm="1">
         <f t="array" aca="1" ref="BK59" ca="1">BY26*$C26*$L26*POWER($F26,$O26)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A21),9))</f>
-        <v>0</v>
+        <v>146.33698473728819</v>
       </c>
       <c r="BL59" s="16" cm="1">
         <f t="array" aca="1" ref="BL59" ca="1">BZ26*$C26*$L26*POWER($F26,$O26)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B21),9))</f>
@@ -39987,11 +39988,11 @@
       </c>
       <c r="BO59" s="16" cm="1">
         <f t="array" aca="1" ref="BO59" ca="1">CC26*$C26*$L26*POWER($F26,$O26)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E21),9))</f>
-        <v>186.64177568163981</v>
+        <v>0</v>
       </c>
       <c r="BP59" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>186.64177568163981</v>
+        <v>146.33698473728819</v>
       </c>
       <c r="BQ59" s="8"/>
       <c r="BR59" s="8"/>
@@ -40084,7 +40085,7 @@
       </c>
       <c r="BK60" s="61" cm="1">
         <f t="array" aca="1" ref="BK60" ca="1">BY27*$C27*$L27*POWER($F27,$O27)*INDIRECT(ADDRESS(32+COLUMNS($A$1:A22),9))</f>
-        <v>53.577862653738528</v>
+        <v>0</v>
       </c>
       <c r="BL60" s="16" cm="1">
         <f t="array" aca="1" ref="BL60" ca="1">BZ27*$C27*$L27*POWER($F27,$O27)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B22),9))</f>
@@ -40100,7 +40101,7 @@
       </c>
       <c r="BO60" s="16" cm="1">
         <f t="array" aca="1" ref="BO60" ca="1">CC27*$C27*$L27*POWER($F27,$O27)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E22),9))</f>
-        <v>0</v>
+        <v>53.577862653738528</v>
       </c>
       <c r="BP60" s="1">
         <f t="shared" ca="1" si="23"/>
@@ -40338,11 +40339,11 @@
       </c>
       <c r="BO62" s="16" cm="1">
         <f t="array" aca="1" ref="BO62" ca="1">CC29*$C29*$L29*POWER($F29,$O29)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E24),9))</f>
-        <v>41.292619364947292</v>
+        <v>71.894626096254626</v>
       </c>
       <c r="BP62" s="1">
         <f t="shared" ca="1" si="23"/>
-        <v>41.292619364947292</v>
+        <v>71.894626096254626</v>
       </c>
       <c r="BQ62" s="8"/>
       <c r="BR62" s="8"/>
@@ -40409,7 +40410,7 @@
       <c r="Q63" s="8"/>
       <c r="R63" s="8" cm="1">
         <f t="array" aca="1" ref="R63" ca="1">-C33+SUM(INDIRECT(ADDRESS(6,69+ROWS($A$1:A1))):INDIRECT(ADDRESS(30,69+ROWS($A$1:A1)))*$F$6:$F$30)</f>
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="S63" s="8" t="s">
         <v>21</v>
@@ -40501,7 +40502,7 @@
       </c>
       <c r="BL63" s="16" cm="1">
         <f t="array" aca="1" ref="BL63" ca="1">BZ30*$C30*$L30*POWER($F30,$O30)*INDIRECT(ADDRESS(32+COLUMNS($A$1:B25),9))</f>
-        <v>0</v>
+        <v>1317.3966981156575</v>
       </c>
       <c r="BM63" s="16" cm="1">
         <f t="array" aca="1" ref="BM63" ca="1">CA30*$C30*$L30*POWER($F30,$O30)*INDIRECT(ADDRESS(32+COLUMNS($A$1:C25),9))</f>
@@ -40509,7 +40510,7 @@
       </c>
       <c r="BN63" s="16" cm="1">
         <f t="array" aca="1" ref="BN63" ca="1">CB30*$C30*$L30*POWER($F30,$O30)*INDIRECT(ADDRESS(32+COLUMNS($A$1:D25),9))</f>
-        <v>1317.3966981156575</v>
+        <v>0</v>
       </c>
       <c r="BO63" s="16" cm="1">
         <f t="array" aca="1" ref="BO63" ca="1">CC30*$C30*$L30*POWER($F30,$O30)*INDIRECT(ADDRESS(32+COLUMNS($A$1:E25),9))</f>
@@ -40584,7 +40585,7 @@
       <c r="Q64" s="8"/>
       <c r="R64" s="8" cm="1">
         <f t="array" aca="1" ref="R64" ca="1">-C34+SUM(INDIRECT(ADDRESS(6,69+ROWS($A$1:A2))):INDIRECT(ADDRESS(30,69+ROWS($A$1:A2)))*$F$6:$F$30)</f>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="S64" s="8" t="s">
         <v>21</v>
@@ -40608,7 +40609,7 @@
       <c r="AA64" s="8"/>
       <c r="AB64" s="8" cm="1">
         <f t="array" aca="1" ref="AB64" ca="1">INDIRECT(ADDRESS(5+$B43,62+COLUMNS($A2:A2)))+INDIRECT(ADDRESS(5+$C43,62+COLUMNS($A2:A2)))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC64" s="8" cm="1">
         <f t="array" aca="1" ref="AC64" ca="1">INDIRECT(ADDRESS(5+$B43,62+COLUMNS($A2:B2)))+INDIRECT(ADDRESS(5+$C43,62+COLUMNS($A2:B2)))</f>
@@ -40624,7 +40625,7 @@
       </c>
       <c r="AF64" s="8" cm="1">
         <f t="array" aca="1" ref="AF64" ca="1">INDIRECT(ADDRESS(5+$B43,62+COLUMNS($A2:E2)))+INDIRECT(ADDRESS(5+$C43,62+COLUMNS($A2:E2)))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AG64" s="8" t="s">
         <v>21</v>
@@ -40672,27 +40673,27 @@
       </c>
       <c r="BK64" s="8">
         <f ca="1">SUM(BK39:BK63)</f>
-        <v>178.93554447148782</v>
+        <v>175.50066263599186</v>
       </c>
       <c r="BL64" s="8">
         <f t="shared" ref="BL64:BO64" ca="1" si="25">SUM(BL39:BL63)</f>
-        <v>1105.5380709689553</v>
+        <v>1317.3966981156575</v>
       </c>
       <c r="BM64" s="8">
         <f t="shared" ca="1" si="25"/>
-        <v>3508.4675608847338</v>
+        <v>3512.1389595578294</v>
       </c>
       <c r="BN64" s="8">
         <f t="shared" ca="1" si="25"/>
-        <v>1800.3550364325747</v>
+        <v>1588.4964092858727</v>
       </c>
       <c r="BO64" s="8">
         <f t="shared" ca="1" si="25"/>
-        <v>345.052834091872</v>
+        <v>352.20078962360418</v>
       </c>
       <c r="BP64" s="59">
         <f t="shared" ca="1" si="23"/>
-        <v>6938.3490468496238</v>
+        <v>6945.7335192189557</v>
       </c>
       <c r="BQ64" s="8" t="s">
         <v>1168</v>
@@ -40892,7 +40893,7 @@
       <c r="G66" s="8"/>
       <c r="H66" s="8" cm="1">
         <f t="array" ref="H66">SUM(AA9:AE9*BR9:BV9-R9*BK9:BO9)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I66" s="8" t="s">
         <v>25</v>
@@ -40904,7 +40905,7 @@
       <c r="L66" s="8"/>
       <c r="M66" s="8" cm="1">
         <f t="array" ref="M66">SUM(AA9:AE9*BR9:BV9-U9*BK9:BO9)</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="N66" s="8" t="s">
         <v>21</v>
@@ -40916,7 +40917,7 @@
       <c r="Q66" s="8"/>
       <c r="R66" s="8" cm="1">
         <f t="array" aca="1" ref="R66" ca="1">-C36+SUM(INDIRECT(ADDRESS(6,69+ROWS($A$1:A4))):INDIRECT(ADDRESS(30,69+ROWS($A$1:A4)))*$F$6:$F$30)</f>
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="S66" s="8" t="s">
         <v>21</v>
@@ -41129,7 +41130,7 @@
       <c r="B68" s="10"/>
       <c r="C68" s="8">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D68" s="8" t="s">
         <v>21</v>
@@ -41141,7 +41142,7 @@
       <c r="G68" s="8"/>
       <c r="H68" s="8" cm="1">
         <f t="array" ref="H68">SUM(AA11:AE11*BR11:BV11-R11*BK11:BO11)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="I68" s="8" t="s">
         <v>25</v>
@@ -41153,7 +41154,7 @@
       <c r="L68" s="8"/>
       <c r="M68" s="8" cm="1">
         <f t="array" ref="M68">SUM(AA11:AE11*BR11:BV11-U11*BK11:BO11)</f>
-        <v>0</v>
+        <v>-18</v>
       </c>
       <c r="N68" s="8" t="s">
         <v>21</v>
@@ -41711,7 +41712,7 @@
       <c r="G73" s="8"/>
       <c r="H73" s="8" cm="1">
         <f t="array" ref="H73">SUM(AA16:AE16*BR16:BV16-R16*BK16:BO16)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="I73" s="8" t="s">
         <v>25</v>
@@ -41723,7 +41724,7 @@
       <c r="L73" s="8"/>
       <c r="M73" s="8" cm="1">
         <f t="array" ref="M73">SUM(AA16:AE16*BR16:BV16-U16*BK16:BO16)</f>
-        <v>-12</v>
+        <v>-11</v>
       </c>
       <c r="N73" s="8" t="s">
         <v>21</v>
@@ -42842,7 +42843,7 @@
       <c r="G83" s="8"/>
       <c r="H83" s="8" cm="1">
         <f t="array" ref="H83">SUM(AA26:AE26*BR26:BV26-R26*BK26:BO26)</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I83" s="8" t="s">
         <v>25</v>
@@ -42854,7 +42855,7 @@
       <c r="L83" s="8"/>
       <c r="M83" s="8" cm="1">
         <f t="array" ref="M83">SUM(AA26:AE26*BR26:BV26-U26*BK26:BO26)</f>
-        <v>-15</v>
+        <v>-16</v>
       </c>
       <c r="N83" s="8" t="s">
         <v>21</v>
@@ -43183,7 +43184,7 @@
       <c r="G86" s="8"/>
       <c r="H86" s="8" cm="1">
         <f t="array" ref="H86">SUM(AA29:AE29*BR29:BV29-R29*BK29:BO29)</f>
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="I86" s="8" t="s">
         <v>25</v>
@@ -43195,7 +43196,7 @@
       <c r="L86" s="8"/>
       <c r="M86" s="8" cm="1">
         <f t="array" ref="M86">SUM(AA29:AE29*BR29:BV29-U29*BK29:BO29)</f>
-        <v>-11</v>
+        <v>-6</v>
       </c>
       <c r="N86" s="8" t="s">
         <v>21</v>
@@ -43297,7 +43298,7 @@
       <c r="G87" s="8"/>
       <c r="H87" s="8" cm="1">
         <f t="array" ref="H87">SUM(AA30:AE30*BR30:BV30-R30*BK30:BO30)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="I87" s="8" t="s">
         <v>25</v>
@@ -43309,7 +43310,7 @@
       <c r="L87" s="8"/>
       <c r="M87" s="8" cm="1">
         <f t="array" ref="M87">SUM(AA30:AE30*BR30:BV30-U30*BK30:BO30)</f>
-        <v>-6</v>
+        <v>-2</v>
       </c>
       <c r="N87" s="8" t="s">
         <v>21</v>
@@ -45398,12 +45399,9 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -45539,15 +45537,26 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7F82F3A-971A-4E00-BEE7-5E3A8CB8E835}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9105EF9-87DC-400D-AF3A-CEFE01235C70}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="b79073fe-1e48-4a97-9229-baaa8603d156"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -45571,17 +45580,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E9105EF9-87DC-400D-AF3A-CEFE01235C70}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D7F82F3A-971A-4E00-BEE7-5E3A8CB8E835}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="b79073fe-1e48-4a97-9229-baaa8603d156"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>